<commit_message>
Regenerate talenox column headers
</commit_message>
<xml_diff>
--- a/data/tlx_import_sheet_samples/malaysia.xlsx
+++ b/data/tlx_import_sheet_samples/malaysia.xlsx
@@ -29,13 +29,13 @@
     <definedName name="Banten" localSheetId="0">'ReferenceValues'!$C$2:$C$9</definedName>
     <definedName name="Bengkulu" localSheetId="0">'ReferenceValues'!$D$2:$D$11</definedName>
     <definedName name="Gorontalo" localSheetId="0">'ReferenceValues'!$E$2:$E$7</definedName>
-    <definedName name="DKIJakarta" localSheetId="0">'ReferenceValues'!$F$2:$F$7</definedName>
-    <definedName name="Jambi" localSheetId="0">'ReferenceValues'!$G$2:$G$12</definedName>
-    <definedName name="JawaBarat" localSheetId="0">'ReferenceValues'!$H$2:$H$28</definedName>
-    <definedName name="JawaTengah" localSheetId="0">'ReferenceValues'!$I$2:$I$36</definedName>
-    <definedName name="JawaTimur" localSheetId="0">'ReferenceValues'!$J$2:$J$36</definedName>
-    <definedName name="KalimantanBarat" localSheetId="0">'ReferenceValues'!$K$2:$K$15</definedName>
-    <definedName name="KalimantanUtara" localSheetId="0">'ReferenceValues'!$L$2:$L$6</definedName>
+    <definedName name="PapuaBarat" localSheetId="0">'ReferenceValues'!$F$2:$F$14</definedName>
+    <definedName name="DKIJakarta" localSheetId="0">'ReferenceValues'!$G$2:$G$7</definedName>
+    <definedName name="Jambi" localSheetId="0">'ReferenceValues'!$H$2:$H$12</definedName>
+    <definedName name="JawaBarat" localSheetId="0">'ReferenceValues'!$I$2:$I$28</definedName>
+    <definedName name="JawaTengah" localSheetId="0">'ReferenceValues'!$J$2:$J$36</definedName>
+    <definedName name="JawaTimur" localSheetId="0">'ReferenceValues'!$K$2:$K$36</definedName>
+    <definedName name="KalimantanBarat" localSheetId="0">'ReferenceValues'!$L$2:$L$15</definedName>
     <definedName name="KalimantanSelatan" localSheetId="0">'ReferenceValues'!$M$2:$M$14</definedName>
     <definedName name="KalimantanTengah" localSheetId="0">'ReferenceValues'!$N$2:$N$15</definedName>
     <definedName name="KalimantanTimur" localSheetId="0">'ReferenceValues'!$O$2:$O$11</definedName>
@@ -47,17 +47,17 @@
     <definedName name="NusaTenggaraBarat" localSheetId="0">'ReferenceValues'!$U$2:$U$11</definedName>
     <definedName name="NusaTenggaraTimur" localSheetId="0">'ReferenceValues'!$V$2:$V$23</definedName>
     <definedName name="Papua" localSheetId="0">'ReferenceValues'!$W$2:$W$30</definedName>
-    <definedName name="PapuaBarat" localSheetId="0">'ReferenceValues'!$X$2:$X$14</definedName>
-    <definedName name="Riau" localSheetId="0">'ReferenceValues'!$Y$2:$Y$13</definedName>
-    <definedName name="SulawesiBarat" localSheetId="0">'ReferenceValues'!$Z$2:$Z$7</definedName>
-    <definedName name="SulawesiSelatan" localSheetId="0">'ReferenceValues'!$AA$2:$AA$25</definedName>
-    <definedName name="SulawesiTengah" localSheetId="0">'ReferenceValues'!$AB$2:$AB$14</definedName>
-    <definedName name="SulawesiTenggara" localSheetId="0">'ReferenceValues'!$AC$2:$AC$18</definedName>
-    <definedName name="SulawesiUtara" localSheetId="0">'ReferenceValues'!$AD$2:$AD$6</definedName>
-    <definedName name="SumateraBarat" localSheetId="0">'ReferenceValues'!$AE$2:$AE$20</definedName>
-    <definedName name="SumateraSelatan" localSheetId="0">'ReferenceValues'!$AF$2:$AF$18</definedName>
-    <definedName name="SumateraUtara" localSheetId="0">'ReferenceValues'!$AG$2:$AG$34</definedName>
-    <definedName name="Yogyakarta" localSheetId="0">'ReferenceValues'!$AH$2:$AH$6</definedName>
+    <definedName name="Riau" localSheetId="0">'ReferenceValues'!$X$2:$X$13</definedName>
+    <definedName name="SulawesiBarat" localSheetId="0">'ReferenceValues'!$Y$2:$Y$7</definedName>
+    <definedName name="SulawesiSelatan" localSheetId="0">'ReferenceValues'!$Z$2:$Z$25</definedName>
+    <definedName name="SulawesiTengah" localSheetId="0">'ReferenceValues'!$AA$2:$AA$14</definedName>
+    <definedName name="SulawesiTenggara" localSheetId="0">'ReferenceValues'!$AB$2:$AB$18</definedName>
+    <definedName name="SulawesiUtara" localSheetId="0">'ReferenceValues'!$AC$2:$AC$6</definedName>
+    <definedName name="SumateraBarat" localSheetId="0">'ReferenceValues'!$AD$2:$AD$20</definedName>
+    <definedName name="SumateraSelatan" localSheetId="0">'ReferenceValues'!$AE$2:$AE$18</definedName>
+    <definedName name="SumateraUtara" localSheetId="0">'ReferenceValues'!$AF$2:$AF$34</definedName>
+    <definedName name="Yogyakarta" localSheetId="0">'ReferenceValues'!$AG$2:$AG$6</definedName>
+    <definedName name="KalimantanUtara" localSheetId="0">'ReferenceValues'!$AH$2:$AH$6</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="T4" s="15" t="inlineStr">
         <is>
-          <t>Married and Spouse Not Working</t>
+          <t>Divorce/Widow/Widower</t>
         </is>
       </c>
       <c r="U4" s="15" t="inlineStr">
@@ -1989,12 +1989,12 @@
       </c>
       <c r="AA4" s="15" t="inlineStr">
         <is>
-          <t>28%</t>
+          <t>17%</t>
         </is>
       </c>
       <c r="AB4" s="15" t="inlineStr">
         <is>
-          <t>5.5%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="AC4" s="15" t="inlineStr">
@@ -2064,7 +2064,7 @@
       </c>
       <c r="AP4" s="15" t="inlineStr">
         <is>
-          <t>Taoism</t>
+          <t>Christianity</t>
         </is>
       </c>
       <c r="AQ4" s="15" t="inlineStr">
@@ -2119,7 +2119,7 @@
       </c>
       <c r="BA4" s="15" t="inlineStr">
         <is>
-          <t>Hourly</t>
+          <t>Monthly</t>
         </is>
       </c>
       <c r="BB4" s="15" t="inlineStr">
@@ -2294,17 +2294,17 @@
       </c>
       <c r="CR4" s="15" t="inlineStr">
         <is>
-          <t>August</t>
+          <t>July</t>
         </is>
       </c>
       <c r="CS4" s="15" t="inlineStr">
         <is>
-          <t>Not Vaccinated</t>
+          <t>Fully Vaccinated</t>
         </is>
       </c>
       <c r="CT4" s="15" t="inlineStr">
         <is>
-          <t>Johnson &amp; Johnson Janssen</t>
+          <t>Moderna</t>
         </is>
       </c>
       <c r="CU4" s="15" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="CW4" s="15" t="inlineStr">
         <is>
-          <t>Oxford-AstraZeneca</t>
+          <t>Sinovac-CoronaVac</t>
         </is>
       </c>
       <c r="CX4" s="15" t="inlineStr">
@@ -2388,13 +2388,13 @@
       <formula1>DataValidation!G$1:G$3</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="BB3:BB1048576">
-      <formula1>DataValidation!H$1:H$34</formula1>
+      <formula1>DataValidation!H$1:H$35</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="BG3:BG1048576">
       <formula1>DataValidation!I$1:I$3</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="BH3:BH1048576">
-      <formula1>DataValidation!J$1:J$37</formula1>
+      <formula1>DataValidation!J$1:J$38</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="BY3:BY1048576">
       <formula1>DataValidation!K$1:K$9</formula1>
@@ -2529,7 +2529,7 @@
       <formula1>DataValidation!AY$1:AY$24</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="AE3:AE1048576">
-      <formula1>DataValidation!AZ$1:AZ$4</formula1>
+      <formula1>DataValidation!AZ$1:AZ$5</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="stop" allowBlank="1" showDropDown="false" showInputMessage="1" showErrorMessage="1" errorTitle="" error="Please choose a valid option" promptTitle="" prompt="" sqref="AI3:AI1048576">
       <formula1>DataValidation!A$1:A$2</formula1>
@@ -3091,7 +3091,7 @@
       </c>
       <c r="AZ2" s="0" t="inlineStr">
         <is>
-          <t>Employment Injury Scheme and Invalidity Scheme</t>
+          <t>Automatic scheme selection based on age</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="AZ3" s="0" t="inlineStr">
         <is>
-          <t>Employment Injury Scheme</t>
+          <t>Employment Injury Scheme and Invalidity Scheme</t>
         </is>
       </c>
     </row>
@@ -3349,7 +3349,7 @@
       <c r="I4" s="0"/>
       <c r="J4" s="0" t="inlineStr">
         <is>
-          <t>Public Bank</t>
+          <t>HSBC Amanah Malaysia</t>
         </is>
       </c>
       <c r="K4" s="0" t="inlineStr">
@@ -3507,11 +3507,11 @@
       </c>
       <c r="AZ4" s="0" t="inlineStr">
         <is>
-          <t>Foreign Workers Social Security</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" spans="1:51" customFormat="false">
+          <t>Employment Injury Scheme</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:52" customFormat="false">
       <c r="A5" s="0"/>
       <c r="B5" s="0"/>
       <c r="C5" s="0"/>
@@ -3539,7 +3539,7 @@
       <c r="I5" s="0"/>
       <c r="J5" s="0" t="inlineStr">
         <is>
-          <t>Maybank</t>
+          <t>Public Bank</t>
         </is>
       </c>
       <c r="K5" s="0" t="inlineStr">
@@ -3675,6 +3675,11 @@
           <t>12%</t>
         </is>
       </c>
+      <c r="AZ5" s="0" t="inlineStr">
+        <is>
+          <t>Foreign Workers Social Security</t>
+        </is>
+      </c>
     </row>
     <row r="6" spans="1:51" customFormat="false">
       <c r="A6" s="0"/>
@@ -3704,7 +3709,7 @@
       <c r="I6" s="0"/>
       <c r="J6" s="0" t="inlineStr">
         <is>
-          <t>CIMB</t>
+          <t>Maybank</t>
         </is>
       </c>
       <c r="K6" s="0" t="inlineStr">
@@ -3869,7 +3874,7 @@
       <c r="I7" s="0"/>
       <c r="J7" s="0" t="inlineStr">
         <is>
-          <t>RHB</t>
+          <t>CIMB</t>
         </is>
       </c>
       <c r="K7" s="0" t="inlineStr">
@@ -4034,7 +4039,7 @@
       <c r="I8" s="0"/>
       <c r="J8" s="0" t="inlineStr">
         <is>
-          <t>AmInvestment Bank</t>
+          <t>RHB</t>
         </is>
       </c>
       <c r="K8" s="0" t="inlineStr">
@@ -4199,7 +4204,7 @@
       <c r="I9" s="0"/>
       <c r="J9" s="0" t="inlineStr">
         <is>
-          <t>UOB</t>
+          <t>AmInvestment Bank</t>
         </is>
       </c>
       <c r="K9" s="0" t="inlineStr">
@@ -4348,7 +4353,7 @@
       <c r="I10" s="0"/>
       <c r="J10" s="0" t="inlineStr">
         <is>
-          <t>Bank Rakyat</t>
+          <t>UOB</t>
         </is>
       </c>
       <c r="K10" s="0"/>
@@ -4493,7 +4498,7 @@
       <c r="I11" s="0"/>
       <c r="J11" s="0" t="inlineStr">
         <is>
-          <t>OCBC</t>
+          <t>Bank Rakyat</t>
         </is>
       </c>
       <c r="K11" s="0"/>
@@ -4634,7 +4639,7 @@
       <c r="I12" s="0"/>
       <c r="J12" s="0" t="inlineStr">
         <is>
-          <t>HSBC</t>
+          <t>OCBC</t>
         </is>
       </c>
       <c r="K12" s="0"/>
@@ -4775,7 +4780,7 @@
       <c r="I13" s="0"/>
       <c r="J13" s="0" t="inlineStr">
         <is>
-          <t>Standard Chartered</t>
+          <t>HSBC</t>
         </is>
       </c>
       <c r="K13" s="0"/>
@@ -4912,7 +4917,7 @@
       <c r="I14" s="0"/>
       <c r="J14" s="0" t="inlineStr">
         <is>
-          <t>Citibank</t>
+          <t>Standard Chartered</t>
         </is>
       </c>
       <c r="K14" s="0"/>
@@ -5045,7 +5050,7 @@
       <c r="I15" s="0"/>
       <c r="J15" s="0" t="inlineStr">
         <is>
-          <t>AmBank</t>
+          <t>Citibank</t>
         </is>
       </c>
       <c r="K15" s="0"/>
@@ -5174,7 +5179,7 @@
       <c r="I16" s="0"/>
       <c r="J16" s="0" t="inlineStr">
         <is>
-          <t>DBS</t>
+          <t>AmBank</t>
         </is>
       </c>
       <c r="K16" s="0"/>
@@ -5299,7 +5304,7 @@
       <c r="I17" s="0"/>
       <c r="J17" s="0" t="inlineStr">
         <is>
-          <t>Bank Islam</t>
+          <t>DBS</t>
         </is>
       </c>
       <c r="K17" s="0"/>
@@ -5420,7 +5425,7 @@
       <c r="I18" s="0"/>
       <c r="J18" s="0" t="inlineStr">
         <is>
-          <t>Affin Bank</t>
+          <t>Bank Islam</t>
         </is>
       </c>
       <c r="K18" s="0"/>
@@ -5541,7 +5546,7 @@
       <c r="I19" s="0"/>
       <c r="J19" s="0" t="inlineStr">
         <is>
-          <t>BSN Bank</t>
+          <t>Affin Bank</t>
         </is>
       </c>
       <c r="K19" s="0"/>
@@ -5662,7 +5667,7 @@
       <c r="I20" s="0"/>
       <c r="J20" s="0" t="inlineStr">
         <is>
-          <t>Alliance Bank</t>
+          <t>BSN Bank</t>
         </is>
       </c>
       <c r="K20" s="0"/>
@@ -5783,7 +5788,7 @@
       <c r="I21" s="0"/>
       <c r="J21" s="0" t="inlineStr">
         <is>
-          <t>Hong Leong Bank</t>
+          <t>Alliance Bank</t>
         </is>
       </c>
       <c r="K21" s="0"/>
@@ -5904,7 +5909,7 @@
       <c r="I22" s="0"/>
       <c r="J22" s="0" t="inlineStr">
         <is>
-          <t>Pakistan - Bank AlHabib</t>
+          <t>Hong Leong Bank</t>
         </is>
       </c>
       <c r="K22" s="0"/>
@@ -6021,7 +6026,7 @@
       <c r="I23" s="0"/>
       <c r="J23" s="0" t="inlineStr">
         <is>
-          <t>Pakistan - Habib Limited Bank</t>
+          <t>Pakistan - Bank AlHabib</t>
         </is>
       </c>
       <c r="K23" s="0"/>
@@ -6138,7 +6143,7 @@
       <c r="I24" s="0"/>
       <c r="J24" s="0" t="inlineStr">
         <is>
-          <t>Bank of China</t>
+          <t>Pakistan - Habib Limited Bank</t>
         </is>
       </c>
       <c r="K24" s="0"/>
@@ -6255,7 +6260,7 @@
       <c r="I25" s="0"/>
       <c r="J25" s="0" t="inlineStr">
         <is>
-          <t>Bank of Tokyo</t>
+          <t>Bank of China</t>
         </is>
       </c>
       <c r="K25" s="0"/>
@@ -6363,7 +6368,7 @@
       <c r="I26" s="0"/>
       <c r="J26" s="0" t="inlineStr">
         <is>
-          <t>Bank Muamalat</t>
+          <t>Bank of Tokyo</t>
         </is>
       </c>
       <c r="K26" s="0"/>
@@ -6471,7 +6476,7 @@
       <c r="I27" s="0"/>
       <c r="J27" s="0" t="inlineStr">
         <is>
-          <t>Bank Pertanian Malaysia Berhad (AGROBANK)</t>
+          <t>Bank Muamalat</t>
         </is>
       </c>
       <c r="K27" s="0"/>
@@ -6579,7 +6584,7 @@
       <c r="I28" s="0"/>
       <c r="J28" s="0" t="inlineStr">
         <is>
-          <t>Bank Simpanan Nasional</t>
+          <t>Bank Pertanian Malaysia Berhad (AGROBANK)</t>
         </is>
       </c>
       <c r="K28" s="0"/>
@@ -6687,7 +6692,7 @@
       <c r="I29" s="0"/>
       <c r="J29" s="0" t="inlineStr">
         <is>
-          <t>BNP PARIBAS</t>
+          <t>Bank Simpanan Nasional</t>
         </is>
       </c>
       <c r="K29" s="0"/>
@@ -6795,7 +6800,7 @@
       <c r="I30" s="0"/>
       <c r="J30" s="0" t="inlineStr">
         <is>
-          <t>DEUTSCHE Bank</t>
+          <t>BNP PARIBAS</t>
         </is>
       </c>
       <c r="K30" s="0"/>
@@ -6892,7 +6897,7 @@
       <c r="I31" s="0"/>
       <c r="J31" s="0" t="inlineStr">
         <is>
-          <t>Industrial and Commercial Bank of China Limited</t>
+          <t>DEUTSCHE Bank</t>
         </is>
       </c>
       <c r="K31" s="0"/>
@@ -6989,7 +6994,7 @@
       <c r="I32" s="0"/>
       <c r="J32" s="0" t="inlineStr">
         <is>
-          <t>JP Morgan Chase Bank Berhad</t>
+          <t>Industrial and Commercial Bank of China Limited</t>
         </is>
       </c>
       <c r="K32" s="0"/>
@@ -7082,7 +7087,7 @@
       <c r="I33" s="0"/>
       <c r="J33" s="0" t="inlineStr">
         <is>
-          <t>Kuwait Finance House</t>
+          <t>JP Morgan Chase Bank Berhad</t>
         </is>
       </c>
       <c r="K33" s="0"/>
@@ -7175,7 +7180,7 @@
       <c r="I34" s="0"/>
       <c r="J34" s="0" t="inlineStr">
         <is>
-          <t>Mizuho Corporate Bank Berhad</t>
+          <t>Kuwait Finance House</t>
         </is>
       </c>
       <c r="K34" s="0"/>
@@ -7260,11 +7265,15 @@
         </is>
       </c>
       <c r="G35" s="0"/>
-      <c r="H35" s="0"/>
+      <c r="H35" s="0" t="inlineStr">
+        <is>
+          <t>MOP</t>
+        </is>
+      </c>
       <c r="I35" s="0"/>
       <c r="J35" s="0" t="inlineStr">
         <is>
-          <t>Sumitomo Mitsui Banking Corporation</t>
+          <t>Mizuho Corporate Bank Berhad</t>
         </is>
       </c>
       <c r="K35" s="0"/>
@@ -7349,7 +7358,7 @@
       <c r="I36" s="0"/>
       <c r="J36" s="0" t="inlineStr">
         <is>
-          <t>Bank of America</t>
+          <t>Sumitomo Mitsui Banking Corporation</t>
         </is>
       </c>
       <c r="K36" s="0"/>
@@ -7430,7 +7439,7 @@
       <c r="I37" s="0"/>
       <c r="J37" s="0" t="inlineStr">
         <is>
-          <t>Maybank - Singapore Branch</t>
+          <t>Bank of America</t>
         </is>
       </c>
       <c r="K37" s="0"/>
@@ -7509,7 +7518,11 @@
       <c r="G38" s="0"/>
       <c r="H38" s="0"/>
       <c r="I38" s="0"/>
-      <c r="J38" s="0"/>
+      <c r="J38" s="0" t="inlineStr">
+        <is>
+          <t>Maybank - Singapore Branch</t>
+        </is>
+      </c>
       <c r="K38" s="0"/>
       <c r="L38" s="0"/>
       <c r="M38" s="0"/>
@@ -18238,13 +18251,13 @@
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.400000000000002" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.400000000000002" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.800000000000004" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.900000000000002" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.900000000000002" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.500000000000004" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.400000000000002" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.800000000000004" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.900000000000002" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.700000000000003" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="29.700000000000003" bestFit="1" customWidth="1"/>
@@ -18257,16 +18270,16 @@
     <col min="22" max="22" width="30.800000000000004" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="28.6" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="27.500000000000004" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="27.500000000000004" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.3" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.500000000000004" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.400000000000002" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="20.900000000000002" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="28.6" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="37.400000000000006" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30.800000000000004" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="25.3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="27.500000000000004" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.400000000000002" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.900000000000002" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="37.400000000000006" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.800000000000004" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.900000000000002" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" customFormat="false">
@@ -18297,147 +18310,147 @@
       </c>
       <c r="F1" s="0" t="inlineStr">
         <is>
+          <t>Papua Barat</t>
+        </is>
+      </c>
+      <c r="G1" s="0" t="inlineStr">
+        <is>
           <t>DKI Jakarta</t>
         </is>
       </c>
-      <c r="G1" s="0" t="inlineStr">
+      <c r="H1" s="0" t="inlineStr">
         <is>
           <t>Jambi</t>
         </is>
       </c>
-      <c r="H1" s="0" t="inlineStr">
+      <c r="I1" s="0" t="inlineStr">
         <is>
           <t>Jawa Barat</t>
         </is>
       </c>
-      <c r="I1" s="0" t="inlineStr">
+      <c r="J1" s="0" t="inlineStr">
         <is>
           <t>Jawa Tengah</t>
         </is>
       </c>
-      <c r="J1" s="0" t="inlineStr">
+      <c r="K1" s="0" t="inlineStr">
         <is>
           <t>Jawa Timur</t>
         </is>
       </c>
-      <c r="K1" s="0" t="inlineStr">
+      <c r="L1" s="0" t="inlineStr">
         <is>
           <t>Kalimantan Barat</t>
         </is>
       </c>
-      <c r="L1" s="0" t="inlineStr">
+      <c r="M1" s="0" t="inlineStr">
+        <is>
+          <t>Kalimantan Selatan</t>
+        </is>
+      </c>
+      <c r="N1" s="0" t="inlineStr">
+        <is>
+          <t>Kalimantan Tengah</t>
+        </is>
+      </c>
+      <c r="O1" s="0" t="inlineStr">
+        <is>
+          <t>Kalimantan Timur</t>
+        </is>
+      </c>
+      <c r="P1" s="0" t="inlineStr">
+        <is>
+          <t>Kepulauan Bangka Belitung</t>
+        </is>
+      </c>
+      <c r="Q1" s="0" t="inlineStr">
+        <is>
+          <t>Kepulauan Riau</t>
+        </is>
+      </c>
+      <c r="R1" s="0" t="inlineStr">
+        <is>
+          <t>Lampung</t>
+        </is>
+      </c>
+      <c r="S1" s="0" t="inlineStr">
+        <is>
+          <t>Maluku</t>
+        </is>
+      </c>
+      <c r="T1" s="0" t="inlineStr">
+        <is>
+          <t>Maluku Utara</t>
+        </is>
+      </c>
+      <c r="U1" s="0" t="inlineStr">
+        <is>
+          <t>Nusa Tenggara Barat</t>
+        </is>
+      </c>
+      <c r="V1" s="0" t="inlineStr">
+        <is>
+          <t>Nusa Tenggara Timur</t>
+        </is>
+      </c>
+      <c r="W1" s="0" t="inlineStr">
+        <is>
+          <t>Papua</t>
+        </is>
+      </c>
+      <c r="X1" s="0" t="inlineStr">
+        <is>
+          <t>Riau</t>
+        </is>
+      </c>
+      <c r="Y1" s="0" t="inlineStr">
+        <is>
+          <t>Sulawesi Barat</t>
+        </is>
+      </c>
+      <c r="Z1" s="0" t="inlineStr">
+        <is>
+          <t>Sulawesi Selatan</t>
+        </is>
+      </c>
+      <c r="AA1" s="0" t="inlineStr">
+        <is>
+          <t>Sulawesi Tengah</t>
+        </is>
+      </c>
+      <c r="AB1" s="0" t="inlineStr">
+        <is>
+          <t>Sulawesi Tenggara</t>
+        </is>
+      </c>
+      <c r="AC1" s="0" t="inlineStr">
+        <is>
+          <t>Sulawesi Utara</t>
+        </is>
+      </c>
+      <c r="AD1" s="0" t="inlineStr">
+        <is>
+          <t>Sumatera Barat</t>
+        </is>
+      </c>
+      <c r="AE1" s="0" t="inlineStr">
+        <is>
+          <t>Sumatera Selatan</t>
+        </is>
+      </c>
+      <c r="AF1" s="0" t="inlineStr">
+        <is>
+          <t>Sumatera Utara</t>
+        </is>
+      </c>
+      <c r="AG1" s="0" t="inlineStr">
+        <is>
+          <t>Yogyakarta</t>
+        </is>
+      </c>
+      <c r="AH1" s="0" t="inlineStr">
         <is>
           <t>Kalimantan Utara</t>
-        </is>
-      </c>
-      <c r="M1" s="0" t="inlineStr">
-        <is>
-          <t>Kalimantan Selatan</t>
-        </is>
-      </c>
-      <c r="N1" s="0" t="inlineStr">
-        <is>
-          <t>Kalimantan Tengah</t>
-        </is>
-      </c>
-      <c r="O1" s="0" t="inlineStr">
-        <is>
-          <t>Kalimantan Timur</t>
-        </is>
-      </c>
-      <c r="P1" s="0" t="inlineStr">
-        <is>
-          <t>Kepulauan Bangka Belitung</t>
-        </is>
-      </c>
-      <c r="Q1" s="0" t="inlineStr">
-        <is>
-          <t>Kepulauan Riau</t>
-        </is>
-      </c>
-      <c r="R1" s="0" t="inlineStr">
-        <is>
-          <t>Lampung</t>
-        </is>
-      </c>
-      <c r="S1" s="0" t="inlineStr">
-        <is>
-          <t>Maluku</t>
-        </is>
-      </c>
-      <c r="T1" s="0" t="inlineStr">
-        <is>
-          <t>Maluku Utara</t>
-        </is>
-      </c>
-      <c r="U1" s="0" t="inlineStr">
-        <is>
-          <t>Nusa Tenggara Barat</t>
-        </is>
-      </c>
-      <c r="V1" s="0" t="inlineStr">
-        <is>
-          <t>Nusa Tenggara Timur</t>
-        </is>
-      </c>
-      <c r="W1" s="0" t="inlineStr">
-        <is>
-          <t>Papua</t>
-        </is>
-      </c>
-      <c r="X1" s="0" t="inlineStr">
-        <is>
-          <t>Papua Barat</t>
-        </is>
-      </c>
-      <c r="Y1" s="0" t="inlineStr">
-        <is>
-          <t>Riau</t>
-        </is>
-      </c>
-      <c r="Z1" s="0" t="inlineStr">
-        <is>
-          <t>Sulawesi Barat</t>
-        </is>
-      </c>
-      <c r="AA1" s="0" t="inlineStr">
-        <is>
-          <t>Sulawesi Selatan</t>
-        </is>
-      </c>
-      <c r="AB1" s="0" t="inlineStr">
-        <is>
-          <t>Sulawesi Tengah</t>
-        </is>
-      </c>
-      <c r="AC1" s="0" t="inlineStr">
-        <is>
-          <t>Sulawesi Tenggara</t>
-        </is>
-      </c>
-      <c r="AD1" s="0" t="inlineStr">
-        <is>
-          <t>Sulawesi Utara</t>
-        </is>
-      </c>
-      <c r="AE1" s="0" t="inlineStr">
-        <is>
-          <t>Sumatera Barat</t>
-        </is>
-      </c>
-      <c r="AF1" s="0" t="inlineStr">
-        <is>
-          <t>Sumatera Selatan</t>
-        </is>
-      </c>
-      <c r="AG1" s="0" t="inlineStr">
-        <is>
-          <t>Sumatera Utara</t>
-        </is>
-      </c>
-      <c r="AH1" s="0" t="inlineStr">
-        <is>
-          <t>Yogyakarta</t>
         </is>
       </c>
     </row>
@@ -18469,147 +18482,147 @@
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
+          <t>Kab. Fakfak</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
           <t>Kab. Kepulauan Seribu</t>
         </is>
       </c>
-      <c r="G2" s="0" t="inlineStr">
+      <c r="H2" s="0" t="inlineStr">
         <is>
           <t>Kab. Kerinci</t>
         </is>
       </c>
-      <c r="H2" s="0" t="inlineStr">
+      <c r="I2" s="0" t="inlineStr">
         <is>
           <t>Kab. Bogor</t>
         </is>
       </c>
-      <c r="I2" s="0" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>Kab. Cilacap</t>
         </is>
       </c>
-      <c r="J2" s="0" t="inlineStr">
+      <c r="K2" s="0" t="inlineStr">
         <is>
           <t>Kab. Pacitan</t>
         </is>
       </c>
-      <c r="K2" s="0" t="inlineStr">
+      <c r="L2" s="0" t="inlineStr">
         <is>
           <t>Kab. Sambas</t>
         </is>
       </c>
-      <c r="L2" s="0" t="inlineStr">
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tanah Laut</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kotawaringin Barat</t>
+        </is>
+      </c>
+      <c r="O2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Paser</t>
+        </is>
+      </c>
+      <c r="P2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bangka</t>
+        </is>
+      </c>
+      <c r="Q2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Karimun</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lampung Barat</t>
+        </is>
+      </c>
+      <c r="S2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Maluku Tenggara Barat</t>
+        </is>
+      </c>
+      <c r="T2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Halmahera Barat</t>
+        </is>
+      </c>
+      <c r="U2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lombok Barat</t>
+        </is>
+      </c>
+      <c r="V2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sumba Barat</t>
+        </is>
+      </c>
+      <c r="W2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Merauke</t>
+        </is>
+      </c>
+      <c r="X2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kuantan Singingi</t>
+        </is>
+      </c>
+      <c r="Y2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Majene</t>
+        </is>
+      </c>
+      <c r="Z2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kepulauan Selayar</t>
+        </is>
+      </c>
+      <c r="AA2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Banggai Kepulauan</t>
+        </is>
+      </c>
+      <c r="AB2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Buton</t>
+        </is>
+      </c>
+      <c r="AC2" s="0" t="inlineStr">
         <is>
           <t>Kab. Malinau</t>
         </is>
       </c>
-      <c r="M2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tanah Laut</t>
-        </is>
-      </c>
-      <c r="N2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kotawaringin Barat</t>
-        </is>
-      </c>
-      <c r="O2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Paser</t>
-        </is>
-      </c>
-      <c r="P2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bangka</t>
-        </is>
-      </c>
-      <c r="Q2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Karimun</t>
-        </is>
-      </c>
-      <c r="R2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lampung Barat</t>
-        </is>
-      </c>
-      <c r="S2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Maluku Tenggara Barat</t>
-        </is>
-      </c>
-      <c r="T2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Halmahera Barat</t>
-        </is>
-      </c>
-      <c r="U2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lombok Barat</t>
-        </is>
-      </c>
-      <c r="V2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Sumba Barat</t>
-        </is>
-      </c>
-      <c r="W2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Merauke</t>
-        </is>
-      </c>
-      <c r="X2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Fakfak</t>
-        </is>
-      </c>
-      <c r="Y2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kuantan Singingi</t>
-        </is>
-      </c>
-      <c r="Z2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Majene</t>
-        </is>
-      </c>
-      <c r="AA2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Selayar</t>
-        </is>
-      </c>
-      <c r="AB2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Banggai Kepulauan</t>
-        </is>
-      </c>
-      <c r="AC2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Buton</t>
-        </is>
-      </c>
       <c r="AD2" s="0" t="inlineStr">
         <is>
+          <t>Kab. Kepulauan Mentawai</t>
+        </is>
+      </c>
+      <c r="AE2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Ogan Komering Ulu</t>
+        </is>
+      </c>
+      <c r="AF2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Nias</t>
+        </is>
+      </c>
+      <c r="AG2" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kulon Progo</t>
+        </is>
+      </c>
+      <c r="AH2" s="0" t="inlineStr">
+        <is>
           <t>Kab. Malinau</t>
-        </is>
-      </c>
-      <c r="AE2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Mentawai</t>
-        </is>
-      </c>
-      <c r="AF2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Ogan Komering Ulu</t>
-        </is>
-      </c>
-      <c r="AG2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Nias</t>
-        </is>
-      </c>
-      <c r="AH2" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kulon Progo</t>
         </is>
       </c>
     </row>
@@ -18641,147 +18654,147 @@
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
+          <t>Kab. Kaimana</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
           <t>Jakarta Selatan</t>
         </is>
       </c>
-      <c r="G3" s="0" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
         <is>
           <t>Kab. Merangin</t>
         </is>
       </c>
-      <c r="H3" s="0" t="inlineStr">
+      <c r="I3" s="0" t="inlineStr">
         <is>
           <t>Kab. Sukabumi</t>
         </is>
       </c>
-      <c r="I3" s="0" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>Kab. Banyumas</t>
         </is>
       </c>
-      <c r="J3" s="0" t="inlineStr">
+      <c r="K3" s="0" t="inlineStr">
         <is>
           <t>Kab. Ponorogo</t>
         </is>
       </c>
-      <c r="K3" s="0" t="inlineStr">
+      <c r="L3" s="0" t="inlineStr">
         <is>
           <t>Kab. Bengkayang</t>
         </is>
       </c>
-      <c r="L3" s="0" t="inlineStr">
+      <c r="M3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Baru</t>
+        </is>
+      </c>
+      <c r="N3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kotawaringin Timur</t>
+        </is>
+      </c>
+      <c r="O3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kutai Barat</t>
+        </is>
+      </c>
+      <c r="P3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Belitung</t>
+        </is>
+      </c>
+      <c r="Q3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bintan</t>
+        </is>
+      </c>
+      <c r="R3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tanggamus</t>
+        </is>
+      </c>
+      <c r="S3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Maluku Tenggara</t>
+        </is>
+      </c>
+      <c r="T3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Halmahera Tengah</t>
+        </is>
+      </c>
+      <c r="U3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lombok Tengah</t>
+        </is>
+      </c>
+      <c r="V3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sumba Timur</t>
+        </is>
+      </c>
+      <c r="W3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Jayawijaya</t>
+        </is>
+      </c>
+      <c r="X3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Indragiri Hulu</t>
+        </is>
+      </c>
+      <c r="Y3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Polewali Mandar</t>
+        </is>
+      </c>
+      <c r="Z3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bulukumba</t>
+        </is>
+      </c>
+      <c r="AA3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Banggai</t>
+        </is>
+      </c>
+      <c r="AB3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Muna</t>
+        </is>
+      </c>
+      <c r="AC3" s="0" t="inlineStr">
         <is>
           <t>Kab. Bulungan</t>
         </is>
       </c>
-      <c r="M3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Baru</t>
-        </is>
-      </c>
-      <c r="N3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kotawaringin Timur</t>
-        </is>
-      </c>
-      <c r="O3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kutai Barat</t>
-        </is>
-      </c>
-      <c r="P3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Belitung</t>
-        </is>
-      </c>
-      <c r="Q3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bintan</t>
-        </is>
-      </c>
-      <c r="R3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tanggamus</t>
-        </is>
-      </c>
-      <c r="S3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Maluku Tenggara</t>
-        </is>
-      </c>
-      <c r="T3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Halmahera Tengah</t>
-        </is>
-      </c>
-      <c r="U3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lombok Tengah</t>
-        </is>
-      </c>
-      <c r="V3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Sumba Timur</t>
-        </is>
-      </c>
-      <c r="W3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Jayawijaya</t>
-        </is>
-      </c>
-      <c r="X3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kaimana</t>
-        </is>
-      </c>
-      <c r="Y3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Indragiri Hulu</t>
-        </is>
-      </c>
-      <c r="Z3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Polewali Mandar</t>
-        </is>
-      </c>
-      <c r="AA3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bulukumba</t>
-        </is>
-      </c>
-      <c r="AB3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Banggai</t>
-        </is>
-      </c>
-      <c r="AC3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Muna</t>
-        </is>
-      </c>
       <c r="AD3" s="0" t="inlineStr">
         <is>
+          <t>Kab. Pesisir Selatan</t>
+        </is>
+      </c>
+      <c r="AE3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Ogan Komering Ilir</t>
+        </is>
+      </c>
+      <c r="AF3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Mandailing Natal</t>
+        </is>
+      </c>
+      <c r="AG3" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bantul</t>
+        </is>
+      </c>
+      <c r="AH3" s="0" t="inlineStr">
+        <is>
           <t>Kab. Bulungan</t>
-        </is>
-      </c>
-      <c r="AE3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Pesisir Selatan</t>
-        </is>
-      </c>
-      <c r="AF3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Ogan Komering Ilir</t>
-        </is>
-      </c>
-      <c r="AG3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Mandailing Natal</t>
-        </is>
-      </c>
-      <c r="AH3" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bantul</t>
         </is>
       </c>
     </row>
@@ -18813,147 +18826,147 @@
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
+          <t>Kab. Teluk Wondama</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
           <t>Jakarta Timur</t>
         </is>
       </c>
-      <c r="G4" s="0" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
         <is>
           <t>Kab. Sarolangun</t>
         </is>
       </c>
-      <c r="H4" s="0" t="inlineStr">
+      <c r="I4" s="0" t="inlineStr">
         <is>
           <t>Kab. Cianjur</t>
         </is>
       </c>
-      <c r="I4" s="0" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>Kab. Purbalingga</t>
         </is>
       </c>
-      <c r="J4" s="0" t="inlineStr">
+      <c r="K4" s="0" t="inlineStr">
         <is>
           <t>Kab. Trenggalek</t>
         </is>
       </c>
-      <c r="K4" s="0" t="inlineStr">
+      <c r="L4" s="0" t="inlineStr">
         <is>
           <t>Kab. Landak</t>
         </is>
       </c>
-      <c r="L4" s="0" t="inlineStr">
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Banjar</t>
+        </is>
+      </c>
+      <c r="N4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kapuas</t>
+        </is>
+      </c>
+      <c r="O4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kutai Kartanegara</t>
+        </is>
+      </c>
+      <c r="P4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bangka Barat</t>
+        </is>
+      </c>
+      <c r="Q4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Natuna</t>
+        </is>
+      </c>
+      <c r="R4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lampung Selatan</t>
+        </is>
+      </c>
+      <c r="S4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Maluku Tengah</t>
+        </is>
+      </c>
+      <c r="T4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kepulauan Sula</t>
+        </is>
+      </c>
+      <c r="U4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lombok Timur</t>
+        </is>
+      </c>
+      <c r="V4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kupang</t>
+        </is>
+      </c>
+      <c r="W4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Jayapura</t>
+        </is>
+      </c>
+      <c r="X4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Indragiri Hilir</t>
+        </is>
+      </c>
+      <c r="Y4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Mamasa</t>
+        </is>
+      </c>
+      <c r="Z4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bantaeng</t>
+        </is>
+      </c>
+      <c r="AA4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Morowali</t>
+        </is>
+      </c>
+      <c r="AB4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Konawe</t>
+        </is>
+      </c>
+      <c r="AC4" s="0" t="inlineStr">
         <is>
           <t>Kab. Tana Tidung</t>
         </is>
       </c>
-      <c r="M4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Banjar</t>
-        </is>
-      </c>
-      <c r="N4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kapuas</t>
-        </is>
-      </c>
-      <c r="O4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kutai Kartanegara</t>
-        </is>
-      </c>
-      <c r="P4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bangka Barat</t>
-        </is>
-      </c>
-      <c r="Q4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Natuna</t>
-        </is>
-      </c>
-      <c r="R4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lampung Selatan</t>
-        </is>
-      </c>
-      <c r="S4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Maluku Tengah</t>
-        </is>
-      </c>
-      <c r="T4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Sula</t>
-        </is>
-      </c>
-      <c r="U4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lombok Timur</t>
-        </is>
-      </c>
-      <c r="V4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kupang</t>
-        </is>
-      </c>
-      <c r="W4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Jayapura</t>
-        </is>
-      </c>
-      <c r="X4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Teluk Wondama</t>
-        </is>
-      </c>
-      <c r="Y4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Indragiri Hilir</t>
-        </is>
-      </c>
-      <c r="Z4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Mamasa</t>
-        </is>
-      </c>
-      <c r="AA4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bantaeng</t>
-        </is>
-      </c>
-      <c r="AB4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Morowali</t>
-        </is>
-      </c>
-      <c r="AC4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Konawe</t>
-        </is>
-      </c>
       <c r="AD4" s="0" t="inlineStr">
         <is>
+          <t>Kab. Solok</t>
+        </is>
+      </c>
+      <c r="AE4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Muara Enim</t>
+        </is>
+      </c>
+      <c r="AF4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tapanuli Selatan</t>
+        </is>
+      </c>
+      <c r="AG4" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Gunung Kidul</t>
+        </is>
+      </c>
+      <c r="AH4" s="0" t="inlineStr">
+        <is>
           <t>Kab. Tana Tidung</t>
-        </is>
-      </c>
-      <c r="AE4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Solok</t>
-        </is>
-      </c>
-      <c r="AF4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Muara Enim</t>
-        </is>
-      </c>
-      <c r="AG4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tapanuli Selatan</t>
-        </is>
-      </c>
-      <c r="AH4" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Gunung Kidul</t>
         </is>
       </c>
     </row>
@@ -18985,147 +18998,147 @@
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
+          <t>Kab. Teluk Bintuni</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
           <t>Jakarta Pusat</t>
         </is>
       </c>
-      <c r="G5" s="0" t="inlineStr">
+      <c r="H5" s="0" t="inlineStr">
         <is>
           <t>Kab. Batang Hari</t>
         </is>
       </c>
-      <c r="H5" s="0" t="inlineStr">
+      <c r="I5" s="0" t="inlineStr">
         <is>
           <t>Kab. Bandung</t>
         </is>
       </c>
-      <c r="I5" s="0" t="inlineStr">
+      <c r="J5" s="0" t="inlineStr">
         <is>
           <t>Kab. Banjarnegara</t>
         </is>
       </c>
-      <c r="J5" s="0" t="inlineStr">
+      <c r="K5" s="0" t="inlineStr">
         <is>
           <t>Kab. Tulungagung</t>
         </is>
       </c>
-      <c r="K5" s="0" t="inlineStr">
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t>Kab. Mempawah</t>
         </is>
       </c>
-      <c r="L5" s="0" t="inlineStr">
+      <c r="M5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Barito Kuala</t>
+        </is>
+      </c>
+      <c r="N5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Barito Selatan</t>
+        </is>
+      </c>
+      <c r="O5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kutai Timur</t>
+        </is>
+      </c>
+      <c r="P5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bangka Tengah</t>
+        </is>
+      </c>
+      <c r="Q5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lingga</t>
+        </is>
+      </c>
+      <c r="R5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lampung Timur</t>
+        </is>
+      </c>
+      <c r="S5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Buru</t>
+        </is>
+      </c>
+      <c r="T5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Halmahera Selatan</t>
+        </is>
+      </c>
+      <c r="U5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sumbawa</t>
+        </is>
+      </c>
+      <c r="V5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Timor Tengah Selatan</t>
+        </is>
+      </c>
+      <c r="W5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Nabire</t>
+        </is>
+      </c>
+      <c r="X5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Pelalawan</t>
+        </is>
+      </c>
+      <c r="Y5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Mamuju</t>
+        </is>
+      </c>
+      <c r="Z5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Jeneponto</t>
+        </is>
+      </c>
+      <c r="AA5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Poso</t>
+        </is>
+      </c>
+      <c r="AB5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kolaka</t>
+        </is>
+      </c>
+      <c r="AC5" s="0" t="inlineStr">
         <is>
           <t>Kab. Nunukan</t>
         </is>
       </c>
-      <c r="M5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Barito Kuala</t>
-        </is>
-      </c>
-      <c r="N5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Barito Selatan</t>
-        </is>
-      </c>
-      <c r="O5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kutai Timur</t>
-        </is>
-      </c>
-      <c r="P5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bangka Tengah</t>
-        </is>
-      </c>
-      <c r="Q5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lingga</t>
-        </is>
-      </c>
-      <c r="R5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lampung Timur</t>
-        </is>
-      </c>
-      <c r="S5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Buru</t>
-        </is>
-      </c>
-      <c r="T5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Halmahera Selatan</t>
-        </is>
-      </c>
-      <c r="U5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Sumbawa</t>
-        </is>
-      </c>
-      <c r="V5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Timor Tengah Selatan</t>
-        </is>
-      </c>
-      <c r="W5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Nabire</t>
-        </is>
-      </c>
-      <c r="X5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Teluk Bintuni</t>
-        </is>
-      </c>
-      <c r="Y5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Pelalawan</t>
-        </is>
-      </c>
-      <c r="Z5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Mamuju</t>
-        </is>
-      </c>
-      <c r="AA5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Jeneponto</t>
-        </is>
-      </c>
-      <c r="AB5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Poso</t>
-        </is>
-      </c>
-      <c r="AC5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kolaka</t>
-        </is>
-      </c>
       <c r="AD5" s="0" t="inlineStr">
         <is>
+          <t>Kab. Sijunjung</t>
+        </is>
+      </c>
+      <c r="AE5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lahat</t>
+        </is>
+      </c>
+      <c r="AF5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tapanuli Tengah</t>
+        </is>
+      </c>
+      <c r="AG5" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sleman</t>
+        </is>
+      </c>
+      <c r="AH5" s="0" t="inlineStr">
+        <is>
           <t>Kab. Nunukan</t>
-        </is>
-      </c>
-      <c r="AE5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Sijunjung</t>
-        </is>
-      </c>
-      <c r="AF5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lahat</t>
-        </is>
-      </c>
-      <c r="AG5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tapanuli Tengah</t>
-        </is>
-      </c>
-      <c r="AH5" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Sleman</t>
         </is>
       </c>
     </row>
@@ -19157,151 +19170,151 @@
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
+          <t>Kab. Manokwari</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
           <t>Jakarta Barat</t>
         </is>
       </c>
-      <c r="G6" s="0" t="inlineStr">
+      <c r="H6" s="0" t="inlineStr">
         <is>
           <t>Kab. Muaro Jambi</t>
         </is>
       </c>
-      <c r="H6" s="0" t="inlineStr">
+      <c r="I6" s="0" t="inlineStr">
         <is>
           <t>Kab. Garut</t>
         </is>
       </c>
-      <c r="I6" s="0" t="inlineStr">
+      <c r="J6" s="0" t="inlineStr">
         <is>
           <t>Kab. Kebumen</t>
         </is>
       </c>
-      <c r="J6" s="0" t="inlineStr">
+      <c r="K6" s="0" t="inlineStr">
         <is>
           <t>Kab. Blitar</t>
         </is>
       </c>
-      <c r="K6" s="0" t="inlineStr">
+      <c r="L6" s="0" t="inlineStr">
         <is>
           <t>Kab. Sanggau</t>
         </is>
       </c>
-      <c r="L6" s="0" t="inlineStr">
+      <c r="M6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tapin</t>
+        </is>
+      </c>
+      <c r="N6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Barito Utara</t>
+        </is>
+      </c>
+      <c r="O6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Berau</t>
+        </is>
+      </c>
+      <c r="P6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bangka Selatan</t>
+        </is>
+      </c>
+      <c r="Q6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kepulauan Anambas</t>
+        </is>
+      </c>
+      <c r="R6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lampung Tengah</t>
+        </is>
+      </c>
+      <c r="S6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kepulauan Aru</t>
+        </is>
+      </c>
+      <c r="T6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Halmahera Utara</t>
+        </is>
+      </c>
+      <c r="U6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Dompu</t>
+        </is>
+      </c>
+      <c r="V6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Timor Tengah Utara</t>
+        </is>
+      </c>
+      <c r="W6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Kepulauan Yapen</t>
+        </is>
+      </c>
+      <c r="X6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. SIAK</t>
+        </is>
+      </c>
+      <c r="Y6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Mamuju Utara</t>
+        </is>
+      </c>
+      <c r="Z6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Takalar</t>
+        </is>
+      </c>
+      <c r="AA6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Donggala</t>
+        </is>
+      </c>
+      <c r="AB6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Konawe Selatan</t>
+        </is>
+      </c>
+      <c r="AC6" s="0" t="inlineStr">
         <is>
           <t>Tarakan</t>
         </is>
       </c>
-      <c r="M6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tapin</t>
-        </is>
-      </c>
-      <c r="N6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Barito Utara</t>
-        </is>
-      </c>
-      <c r="O6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Berau</t>
-        </is>
-      </c>
-      <c r="P6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Bangka Selatan</t>
-        </is>
-      </c>
-      <c r="Q6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Anambas</t>
-        </is>
-      </c>
-      <c r="R6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Lampung Tengah</t>
-        </is>
-      </c>
-      <c r="S6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Aru</t>
-        </is>
-      </c>
-      <c r="T6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Halmahera Utara</t>
-        </is>
-      </c>
-      <c r="U6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Dompu</t>
-        </is>
-      </c>
-      <c r="V6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Timor Tengah Utara</t>
-        </is>
-      </c>
-      <c r="W6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Kepulauan Yapen</t>
-        </is>
-      </c>
-      <c r="X6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Manokwari</t>
-        </is>
-      </c>
-      <c r="Y6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. SIAK</t>
-        </is>
-      </c>
-      <c r="Z6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Mamuju Utara</t>
-        </is>
-      </c>
-      <c r="AA6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Takalar</t>
-        </is>
-      </c>
-      <c r="AB6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Donggala</t>
-        </is>
-      </c>
-      <c r="AC6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Konawe Selatan</t>
-        </is>
-      </c>
       <c r="AD6" s="0" t="inlineStr">
         <is>
+          <t>Kab. Tanah Datar</t>
+        </is>
+      </c>
+      <c r="AE6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Musi Rawas</t>
+        </is>
+      </c>
+      <c r="AF6" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tapanuli Utara</t>
+        </is>
+      </c>
+      <c r="AG6" s="0" t="inlineStr">
+        <is>
+          <t>Yogyakarta</t>
+        </is>
+      </c>
+      <c r="AH6" s="0" t="inlineStr">
+        <is>
           <t>Tarakan</t>
         </is>
       </c>
-      <c r="AE6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tanah Datar</t>
-        </is>
-      </c>
-      <c r="AF6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Musi Rawas</t>
-        </is>
-      </c>
-      <c r="AG6" s="0" t="inlineStr">
-        <is>
-          <t>Kab. Tapanuli Utara</t>
-        </is>
-      </c>
-      <c r="AH6" s="0" t="inlineStr">
-        <is>
-          <t>Yogyakarta</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" spans="1:33" customFormat="false">
+    </row>
+    <row r="7" spans="1:32" customFormat="false">
       <c r="A7" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Tengah</t>
@@ -19329,35 +19342,39 @@
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
+          <t>Kab. Sorong Selatan</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
           <t>Jakarta Utara</t>
         </is>
       </c>
-      <c r="G7" s="0" t="inlineStr">
+      <c r="H7" s="0" t="inlineStr">
         <is>
           <t>Kab. Tanjung Jabung Timur</t>
         </is>
       </c>
-      <c r="H7" s="0" t="inlineStr">
+      <c r="I7" s="0" t="inlineStr">
         <is>
           <t>Kab. Tasikmalaya</t>
         </is>
       </c>
-      <c r="I7" s="0" t="inlineStr">
+      <c r="J7" s="0" t="inlineStr">
         <is>
           <t>Kab. Purworejo</t>
         </is>
       </c>
-      <c r="J7" s="0" t="inlineStr">
+      <c r="K7" s="0" t="inlineStr">
         <is>
           <t>Kab. Kediri</t>
         </is>
       </c>
-      <c r="K7" s="0" t="inlineStr">
+      <c r="L7" s="0" t="inlineStr">
         <is>
           <t>Kab. Ketapang</t>
         </is>
       </c>
-      <c r="L7" s="0"/>
       <c r="M7" s="0" t="inlineStr">
         <is>
           <t>Kab. Hulu Sungai Selatan</t>
@@ -19415,52 +19432,47 @@
       </c>
       <c r="X7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Sorong Selatan</t>
+          <t>Kab. Kampar</t>
         </is>
       </c>
       <c r="Y7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Kampar</t>
+          <t>Kab. Mamuju Tengah</t>
         </is>
       </c>
       <c r="Z7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Mamuju Tengah</t>
+          <t>Kab. Gowa</t>
         </is>
       </c>
       <c r="AA7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Gowa</t>
+          <t>Kab. Toli-Toli</t>
         </is>
       </c>
       <c r="AB7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Toli-Toli</t>
-        </is>
-      </c>
-      <c r="AC7" s="0" t="inlineStr">
-        <is>
           <t>Kab. Bombana</t>
         </is>
       </c>
-      <c r="AD7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Padang Pariaman</t>
+        </is>
+      </c>
       <c r="AE7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Padang Pariaman</t>
+          <t>Kab. Musi Banyuasin</t>
         </is>
       </c>
       <c r="AF7" s="0" t="inlineStr">
         <is>
-          <t>Kab. Musi Banyuasin</t>
-        </is>
-      </c>
-      <c r="AG7" s="0" t="inlineStr">
-        <is>
           <t>Kab. Toba Samosir</t>
         </is>
       </c>
     </row>
-    <row r="8" spans="1:33" customFormat="false">
+    <row r="8" spans="1:32" customFormat="false">
       <c r="A8" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Barat</t>
@@ -19482,33 +19494,37 @@
         </is>
       </c>
       <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sorong</t>
+        </is>
+      </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0" t="inlineStr">
         <is>
           <t>Kab. Tanjung Jabung Barat</t>
         </is>
       </c>
-      <c r="H8" s="0" t="inlineStr">
+      <c r="I8" s="0" t="inlineStr">
         <is>
           <t>Kab. Ciamis</t>
         </is>
       </c>
-      <c r="I8" s="0" t="inlineStr">
+      <c r="J8" s="0" t="inlineStr">
         <is>
           <t>Kab. Wonosobo</t>
         </is>
       </c>
-      <c r="J8" s="0" t="inlineStr">
+      <c r="K8" s="0" t="inlineStr">
         <is>
           <t>Kab. Malan</t>
         </is>
       </c>
-      <c r="K8" s="0" t="inlineStr">
+      <c r="L8" s="0" t="inlineStr">
         <is>
           <t>Kab. Sintang</t>
         </is>
       </c>
-      <c r="L8" s="0"/>
       <c r="M8" s="0" t="inlineStr">
         <is>
           <t>Kab. Hulu Sungai Tengah</t>
@@ -19566,48 +19582,43 @@
       </c>
       <c r="X8" s="0" t="inlineStr">
         <is>
-          <t>Kab. Sorong</t>
-        </is>
-      </c>
-      <c r="Y8" s="0" t="inlineStr">
-        <is>
           <t>Kab. Rokan Hulu</t>
         </is>
       </c>
-      <c r="Z8" s="0"/>
+      <c r="Y8" s="0"/>
+      <c r="Z8" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Sinjai</t>
+        </is>
+      </c>
       <c r="AA8" s="0" t="inlineStr">
         <is>
-          <t>Kab. Sinjai</t>
+          <t>Kab. Buol</t>
         </is>
       </c>
       <c r="AB8" s="0" t="inlineStr">
         <is>
-          <t>Kab. Buol</t>
-        </is>
-      </c>
-      <c r="AC8" s="0" t="inlineStr">
-        <is>
           <t>Kab. Wakatobi</t>
         </is>
       </c>
-      <c r="AD8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Agam</t>
+        </is>
+      </c>
       <c r="AE8" s="0" t="inlineStr">
         <is>
-          <t>Kab. Agam</t>
+          <t>Kab. Banyu Asin</t>
         </is>
       </c>
       <c r="AF8" s="0" t="inlineStr">
         <is>
-          <t>Kab. Banyu Asin</t>
-        </is>
-      </c>
-      <c r="AG8" s="0" t="inlineStr">
-        <is>
           <t>Kab. Labuhan Batu</t>
         </is>
       </c>
     </row>
-    <row r="9" spans="1:33" customFormat="false">
+    <row r="9" spans="1:32" customFormat="false">
       <c r="A9" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Besar</t>
@@ -19629,33 +19640,37 @@
         </is>
       </c>
       <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" s="0" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Raja Ampat</t>
+        </is>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0" t="inlineStr">
         <is>
           <t>Kab. Tebo</t>
         </is>
       </c>
-      <c r="H9" s="0" t="inlineStr">
+      <c r="I9" s="0" t="inlineStr">
         <is>
           <t>Kab. Kuningan</t>
         </is>
       </c>
-      <c r="I9" s="0" t="inlineStr">
+      <c r="J9" s="0" t="inlineStr">
         <is>
           <t>Kab. Magelang</t>
         </is>
       </c>
-      <c r="J9" s="0" t="inlineStr">
+      <c r="K9" s="0" t="inlineStr">
         <is>
           <t>Kab. Lumajang</t>
         </is>
       </c>
-      <c r="K9" s="0" t="inlineStr">
+      <c r="L9" s="0" t="inlineStr">
         <is>
           <t>Kab. Kapuas Hulu</t>
         </is>
       </c>
-      <c r="L9" s="0"/>
       <c r="M9" s="0" t="inlineStr">
         <is>
           <t>Kab. Hulu Sungai Utara</t>
@@ -19705,48 +19720,43 @@
       </c>
       <c r="X9" s="0" t="inlineStr">
         <is>
-          <t>Kab. Raja Ampat</t>
-        </is>
-      </c>
-      <c r="Y9" s="0" t="inlineStr">
-        <is>
           <t>Kab. Bengkalis</t>
         </is>
       </c>
-      <c r="Z9" s="0"/>
+      <c r="Y9" s="0"/>
+      <c r="Z9" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Maros</t>
+        </is>
+      </c>
       <c r="AA9" s="0" t="inlineStr">
         <is>
-          <t>Kab. Maros</t>
+          <t>Kab. Parigi Moutong</t>
         </is>
       </c>
       <c r="AB9" s="0" t="inlineStr">
         <is>
-          <t>Kab. Parigi Moutong</t>
-        </is>
-      </c>
-      <c r="AC9" s="0" t="inlineStr">
-        <is>
           <t>Kab. Kolaka Utara</t>
         </is>
       </c>
-      <c r="AD9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Lima Puluh Kota</t>
+        </is>
+      </c>
       <c r="AE9" s="0" t="inlineStr">
         <is>
-          <t>Kab. Lima Puluh Kota</t>
+          <t>Kab. Ogan Komering Ulu Selatan</t>
         </is>
       </c>
       <c r="AF9" s="0" t="inlineStr">
         <is>
-          <t>Kab. Ogan Komering Ulu Selatan</t>
-        </is>
-      </c>
-      <c r="AG9" s="0" t="inlineStr">
-        <is>
           <t>Kab. Asahan</t>
         </is>
       </c>
     </row>
-    <row r="10" spans="1:33" customFormat="false">
+    <row r="10" spans="1:32" customFormat="false">
       <c r="A10" s="0" t="inlineStr">
         <is>
           <t>Kab. Pidie</t>
@@ -19764,33 +19774,37 @@
         </is>
       </c>
       <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Tambrauw</t>
+        </is>
+      </c>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0" t="inlineStr">
         <is>
           <t>Kab. Bungo</t>
         </is>
       </c>
-      <c r="H10" s="0" t="inlineStr">
+      <c r="I10" s="0" t="inlineStr">
         <is>
           <t>Kab. Cirebon</t>
         </is>
       </c>
-      <c r="I10" s="0" t="inlineStr">
+      <c r="J10" s="0" t="inlineStr">
         <is>
           <t>Kab. Boyolali</t>
         </is>
       </c>
-      <c r="J10" s="0" t="inlineStr">
+      <c r="K10" s="0" t="inlineStr">
         <is>
           <t>Kab. Jember</t>
         </is>
       </c>
-      <c r="K10" s="0" t="inlineStr">
+      <c r="L10" s="0" t="inlineStr">
         <is>
           <t>Kab. Sekadau</t>
         </is>
       </c>
-      <c r="L10" s="0"/>
       <c r="M10" s="0" t="inlineStr">
         <is>
           <t>Kab. Tabalong</t>
@@ -19840,48 +19854,43 @@
       </c>
       <c r="X10" s="0" t="inlineStr">
         <is>
-          <t>Kab. Tambrauw</t>
-        </is>
-      </c>
-      <c r="Y10" s="0" t="inlineStr">
-        <is>
           <t>Kab. Rokan Hilir</t>
         </is>
       </c>
-      <c r="Z10" s="0"/>
+      <c r="Y10" s="0"/>
+      <c r="Z10" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Pangkajene Dan Kepulauan</t>
+        </is>
+      </c>
       <c r="AA10" s="0" t="inlineStr">
         <is>
-          <t>Kab. Pangkajene Dan Kepulauan</t>
+          <t>Kab. Tojo Una-Una</t>
         </is>
       </c>
       <c r="AB10" s="0" t="inlineStr">
         <is>
-          <t>Kab. Tojo Una-Una</t>
-        </is>
-      </c>
-      <c r="AC10" s="0" t="inlineStr">
-        <is>
           <t>Kab. Buton Utara</t>
         </is>
       </c>
-      <c r="AD10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Pasaman</t>
+        </is>
+      </c>
       <c r="AE10" s="0" t="inlineStr">
         <is>
-          <t>Kab. Pasaman</t>
+          <t>Kab. Ogan Komering Ulu Timur</t>
         </is>
       </c>
       <c r="AF10" s="0" t="inlineStr">
         <is>
-          <t>Kab. Ogan Komering Ulu Timur</t>
-        </is>
-      </c>
-      <c r="AG10" s="0" t="inlineStr">
-        <is>
           <t>Kab. Simalungun</t>
         </is>
       </c>
     </row>
-    <row r="11" spans="1:33" customFormat="false">
+    <row r="11" spans="1:32" customFormat="false">
       <c r="A11" s="0" t="inlineStr">
         <is>
           <t>Kab. Bireuen</t>
@@ -19895,33 +19904,37 @@
         </is>
       </c>
       <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Maybrat</t>
+        </is>
+      </c>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0" t="inlineStr">
         <is>
           <t>Jambi</t>
         </is>
       </c>
-      <c r="H11" s="0" t="inlineStr">
+      <c r="I11" s="0" t="inlineStr">
         <is>
           <t>Kab. Majalengka</t>
         </is>
       </c>
-      <c r="I11" s="0" t="inlineStr">
+      <c r="J11" s="0" t="inlineStr">
         <is>
           <t>Kab. Klaten</t>
         </is>
       </c>
-      <c r="J11" s="0" t="inlineStr">
+      <c r="K11" s="0" t="inlineStr">
         <is>
           <t>Kab. Banyuwangi</t>
         </is>
       </c>
-      <c r="K11" s="0" t="inlineStr">
+      <c r="L11" s="0" t="inlineStr">
         <is>
           <t>Kab. Melawi</t>
         </is>
       </c>
-      <c r="L11" s="0"/>
       <c r="M11" s="0" t="inlineStr">
         <is>
           <t>Kab. Tanah Bumbu</t>
@@ -19971,48 +19984,43 @@
       </c>
       <c r="X11" s="0" t="inlineStr">
         <is>
-          <t>Kab. Maybrat</t>
-        </is>
-      </c>
-      <c r="Y11" s="0" t="inlineStr">
-        <is>
           <t>Kab. Kepulauan Meranti</t>
         </is>
       </c>
-      <c r="Z11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Barru</t>
+        </is>
+      </c>
       <c r="AA11" s="0" t="inlineStr">
         <is>
-          <t>Kab. Barru</t>
+          <t>Kab. Sigi</t>
         </is>
       </c>
       <c r="AB11" s="0" t="inlineStr">
         <is>
-          <t>Kab. Sigi</t>
-        </is>
-      </c>
-      <c r="AC11" s="0" t="inlineStr">
-        <is>
           <t>Kab. Konawe Utara</t>
         </is>
       </c>
-      <c r="AD11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Solok Selatan</t>
+        </is>
+      </c>
       <c r="AE11" s="0" t="inlineStr">
         <is>
-          <t>Kab. Solok Selatan</t>
+          <t>Kab. Ogan Ilir</t>
         </is>
       </c>
       <c r="AF11" s="0" t="inlineStr">
         <is>
-          <t>Kab. Ogan Ilir</t>
-        </is>
-      </c>
-      <c r="AG11" s="0" t="inlineStr">
-        <is>
           <t>Kab. Dairi</t>
         </is>
       </c>
     </row>
-    <row r="12" spans="1:33" customFormat="false">
+    <row r="12" spans="1:32" customFormat="false">
       <c r="A12" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Utara</t>
@@ -20022,33 +20030,37 @@
       <c r="C12" s="0"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
-      <c r="F12" s="0"/>
-      <c r="G12" s="0" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Manokwari Selatan</t>
+        </is>
+      </c>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0" t="inlineStr">
         <is>
           <t>Sungai Penuh</t>
         </is>
       </c>
-      <c r="H12" s="0" t="inlineStr">
+      <c r="I12" s="0" t="inlineStr">
         <is>
           <t>Kab. Sumedang</t>
         </is>
       </c>
-      <c r="I12" s="0" t="inlineStr">
+      <c r="J12" s="0" t="inlineStr">
         <is>
           <t>Kab. Sukoharjo</t>
         </is>
       </c>
-      <c r="J12" s="0" t="inlineStr">
+      <c r="K12" s="0" t="inlineStr">
         <is>
           <t>Kab. Bondowoso</t>
         </is>
       </c>
-      <c r="K12" s="0" t="inlineStr">
+      <c r="L12" s="0" t="inlineStr">
         <is>
           <t>Kab. Kayong Utara</t>
         </is>
       </c>
-      <c r="L12" s="0"/>
       <c r="M12" s="0" t="inlineStr">
         <is>
           <t>Kab. Balangan</t>
@@ -20086,48 +20098,43 @@
       </c>
       <c r="X12" s="0" t="inlineStr">
         <is>
-          <t>Kab. Manokwari Selatan</t>
-        </is>
-      </c>
-      <c r="Y12" s="0" t="inlineStr">
-        <is>
           <t>Pekanbaru</t>
         </is>
       </c>
-      <c r="Z12" s="0"/>
+      <c r="Y12" s="0"/>
+      <c r="Z12" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Bone</t>
+        </is>
+      </c>
       <c r="AA12" s="0" t="inlineStr">
         <is>
-          <t>Kab. Bone</t>
+          <t>Kab. Banggai Laut</t>
         </is>
       </c>
       <c r="AB12" s="0" t="inlineStr">
         <is>
-          <t>Kab. Banggai Laut</t>
-        </is>
-      </c>
-      <c r="AC12" s="0" t="inlineStr">
-        <is>
           <t>Kab. Kolaka Timur</t>
         </is>
       </c>
-      <c r="AD12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Dharmasraya</t>
+        </is>
+      </c>
       <c r="AE12" s="0" t="inlineStr">
         <is>
-          <t>Kab. Dharmasraya</t>
+          <t>Kab. Empat Lawang</t>
         </is>
       </c>
       <c r="AF12" s="0" t="inlineStr">
         <is>
-          <t>Kab. Empat Lawang</t>
-        </is>
-      </c>
-      <c r="AG12" s="0" t="inlineStr">
-        <is>
           <t>Kab. Karo</t>
         </is>
       </c>
     </row>
-    <row r="13" spans="1:33" customFormat="false">
+    <row r="13" spans="1:32" customFormat="false">
       <c r="A13" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Barat Daya</t>
@@ -20137,29 +20144,33 @@
       <c r="C13" s="0"/>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Pegunungan Arfak</t>
+        </is>
+      </c>
       <c r="G13" s="0"/>
-      <c r="H13" s="0" t="inlineStr">
+      <c r="H13" s="0"/>
+      <c r="I13" s="0" t="inlineStr">
         <is>
           <t>Kab. Indramayu</t>
         </is>
       </c>
-      <c r="I13" s="0" t="inlineStr">
+      <c r="J13" s="0" t="inlineStr">
         <is>
           <t>Kab. Wonogiri</t>
         </is>
       </c>
-      <c r="J13" s="0" t="inlineStr">
+      <c r="K13" s="0" t="inlineStr">
         <is>
           <t>Kab. Situbondo</t>
         </is>
       </c>
-      <c r="K13" s="0" t="inlineStr">
+      <c r="L13" s="0" t="inlineStr">
         <is>
           <t>Kab. Kubu Raya</t>
         </is>
       </c>
-      <c r="L13" s="0"/>
       <c r="M13" s="0" t="inlineStr">
         <is>
           <t>Banjarmasin</t>
@@ -20193,48 +20204,43 @@
       </c>
       <c r="X13" s="0" t="inlineStr">
         <is>
-          <t>Kab. Pegunungan Arfak</t>
-        </is>
-      </c>
-      <c r="Y13" s="0" t="inlineStr">
-        <is>
           <t>Dumai</t>
         </is>
       </c>
-      <c r="Z13" s="0"/>
+      <c r="Y13" s="0"/>
+      <c r="Z13" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Soppeng</t>
+        </is>
+      </c>
       <c r="AA13" s="0" t="inlineStr">
         <is>
-          <t>Kab. Soppeng</t>
+          <t>Kab. Morowali Utara</t>
         </is>
       </c>
       <c r="AB13" s="0" t="inlineStr">
         <is>
-          <t>Kab. Morowali Utara</t>
-        </is>
-      </c>
-      <c r="AC13" s="0" t="inlineStr">
-        <is>
           <t>Kab. Konawe Kepulauan</t>
         </is>
       </c>
-      <c r="AD13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Pasaman Barat</t>
+        </is>
+      </c>
       <c r="AE13" s="0" t="inlineStr">
         <is>
-          <t>Kab. Pasaman Barat</t>
+          <t>Kab. Penukal Abab Lematang Ilir</t>
         </is>
       </c>
       <c r="AF13" s="0" t="inlineStr">
         <is>
-          <t>Kab. Penukal Abab Lematang Ilir</t>
-        </is>
-      </c>
-      <c r="AG13" s="0" t="inlineStr">
-        <is>
           <t>Kab. Deli Serdang</t>
         </is>
       </c>
     </row>
-    <row r="14" spans="1:33" customFormat="false">
+    <row r="14" spans="1:32" customFormat="false">
       <c r="A14" s="0" t="inlineStr">
         <is>
           <t>Kab. Gayo Lues</t>
@@ -20244,29 +20250,33 @@
       <c r="C14" s="0"/>
       <c r="D14" s="0"/>
       <c r="E14" s="0"/>
-      <c r="F14" s="0"/>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>Sorong</t>
+        </is>
+      </c>
       <c r="G14" s="0"/>
-      <c r="H14" s="0" t="inlineStr">
+      <c r="H14" s="0"/>
+      <c r="I14" s="0" t="inlineStr">
         <is>
           <t>Kab. Subang</t>
         </is>
       </c>
-      <c r="I14" s="0" t="inlineStr">
+      <c r="J14" s="0" t="inlineStr">
         <is>
           <t>Kab. Karanganyar</t>
         </is>
       </c>
-      <c r="J14" s="0" t="inlineStr">
+      <c r="K14" s="0" t="inlineStr">
         <is>
           <t>Kab. Probolinggo</t>
         </is>
       </c>
-      <c r="K14" s="0" t="inlineStr">
+      <c r="L14" s="0" t="inlineStr">
         <is>
           <t>Pontianak</t>
         </is>
       </c>
-      <c r="L14" s="0"/>
       <c r="M14" s="0" t="inlineStr">
         <is>
           <t>Banjar Baru</t>
@@ -20298,46 +20308,41 @@
           <t>Kab. Yahukimo</t>
         </is>
       </c>
-      <c r="X14" s="0" t="inlineStr">
-        <is>
-          <t>Sorong</t>
-        </is>
-      </c>
+      <c r="X14" s="0"/>
       <c r="Y14" s="0"/>
-      <c r="Z14" s="0"/>
+      <c r="Z14" s="0" t="inlineStr">
+        <is>
+          <t>Kab. Wajo</t>
+        </is>
+      </c>
       <c r="AA14" s="0" t="inlineStr">
         <is>
-          <t>Kab. Wajo</t>
+          <t>Palu</t>
         </is>
       </c>
       <c r="AB14" s="0" t="inlineStr">
         <is>
-          <t>Palu</t>
-        </is>
-      </c>
-      <c r="AC14" s="0" t="inlineStr">
-        <is>
           <t>Kab. Muna Barat</t>
         </is>
       </c>
-      <c r="AD14" s="0"/>
+      <c r="AC14" s="0"/>
+      <c r="AD14" s="0" t="inlineStr">
+        <is>
+          <t>Padang</t>
+        </is>
+      </c>
       <c r="AE14" s="0" t="inlineStr">
         <is>
-          <t>Padang</t>
+          <t>Kab. Musi Rawas Utara</t>
         </is>
       </c>
       <c r="AF14" s="0" t="inlineStr">
         <is>
-          <t>Kab. Musi Rawas Utara</t>
-        </is>
-      </c>
-      <c r="AG14" s="0" t="inlineStr">
-        <is>
           <t>Kab. Langkat</t>
         </is>
       </c>
     </row>
-    <row r="15" spans="1:33" customFormat="false">
+    <row r="15" spans="1:32" customFormat="false">
       <c r="A15" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Tamiang</t>
@@ -20349,27 +20354,27 @@
       <c r="E15" s="0"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
-      <c r="H15" s="0" t="inlineStr">
+      <c r="H15" s="0"/>
+      <c r="I15" s="0" t="inlineStr">
         <is>
           <t>Kab. Purwakarta</t>
         </is>
       </c>
-      <c r="I15" s="0" t="inlineStr">
+      <c r="J15" s="0" t="inlineStr">
         <is>
           <t>Kab. Sragen</t>
         </is>
       </c>
-      <c r="J15" s="0" t="inlineStr">
+      <c r="K15" s="0" t="inlineStr">
         <is>
           <t>Kab. Pasuruan</t>
         </is>
       </c>
-      <c r="K15" s="0" t="inlineStr">
+      <c r="L15" s="0" t="inlineStr">
         <is>
           <t>Singkawang</t>
         </is>
       </c>
-      <c r="L15" s="0"/>
       <c r="M15" s="0"/>
       <c r="N15" s="0" t="inlineStr">
         <is>
@@ -20399,36 +20404,35 @@
       </c>
       <c r="X15" s="0"/>
       <c r="Y15" s="0"/>
-      <c r="Z15" s="0"/>
-      <c r="AA15" s="0" t="inlineStr">
+      <c r="Z15" s="0" t="inlineStr">
         <is>
           <t>Kab. Sidenreng Rappang</t>
         </is>
       </c>
-      <c r="AB15" s="0"/>
-      <c r="AC15" s="0" t="inlineStr">
+      <c r="AA15" s="0"/>
+      <c r="AB15" s="0" t="inlineStr">
         <is>
           <t>Kab. Buton Tengah</t>
         </is>
       </c>
-      <c r="AD15" s="0"/>
+      <c r="AC15" s="0"/>
+      <c r="AD15" s="0" t="inlineStr">
+        <is>
+          <t>Solok</t>
+        </is>
+      </c>
       <c r="AE15" s="0" t="inlineStr">
         <is>
-          <t>Solok</t>
+          <t>Palembang</t>
         </is>
       </c>
       <c r="AF15" s="0" t="inlineStr">
         <is>
-          <t>Palembang</t>
-        </is>
-      </c>
-      <c r="AG15" s="0" t="inlineStr">
-        <is>
           <t>Kab. Nias Selatan</t>
         </is>
       </c>
     </row>
-    <row r="16" spans="1:33" customFormat="false">
+    <row r="16" spans="1:32" customFormat="false">
       <c r="A16" s="0" t="inlineStr">
         <is>
           <t>Kab. Nagan Raya</t>
@@ -20440,22 +20444,22 @@
       <c r="E16" s="0"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
-      <c r="H16" s="0" t="inlineStr">
+      <c r="H16" s="0"/>
+      <c r="I16" s="0" t="inlineStr">
         <is>
           <t>Kab. Karawang</t>
         </is>
       </c>
-      <c r="I16" s="0" t="inlineStr">
+      <c r="J16" s="0" t="inlineStr">
         <is>
           <t>Kab. Grobogan</t>
         </is>
       </c>
-      <c r="J16" s="0" t="inlineStr">
+      <c r="K16" s="0" t="inlineStr">
         <is>
           <t>Kab. Sidoarjo</t>
         </is>
       </c>
-      <c r="K16" s="0"/>
       <c r="L16" s="0"/>
       <c r="M16" s="0"/>
       <c r="N16" s="0"/>
@@ -20482,36 +20486,35 @@
       </c>
       <c r="X16" s="0"/>
       <c r="Y16" s="0"/>
-      <c r="Z16" s="0"/>
-      <c r="AA16" s="0" t="inlineStr">
+      <c r="Z16" s="0" t="inlineStr">
         <is>
           <t>Kab. Pinrang</t>
         </is>
       </c>
-      <c r="AB16" s="0"/>
-      <c r="AC16" s="0" t="inlineStr">
+      <c r="AA16" s="0"/>
+      <c r="AB16" s="0" t="inlineStr">
         <is>
           <t>Kab. Buton Selatan</t>
         </is>
       </c>
-      <c r="AD16" s="0"/>
+      <c r="AC16" s="0"/>
+      <c r="AD16" s="0" t="inlineStr">
+        <is>
+          <t>Sawah Lunto</t>
+        </is>
+      </c>
       <c r="AE16" s="0" t="inlineStr">
         <is>
-          <t>Sawah Lunto</t>
+          <t>Prabumulih</t>
         </is>
       </c>
       <c r="AF16" s="0" t="inlineStr">
         <is>
-          <t>Prabumulih</t>
-        </is>
-      </c>
-      <c r="AG16" s="0" t="inlineStr">
-        <is>
           <t>Kab. Humbang Hasundutan</t>
         </is>
       </c>
     </row>
-    <row r="17" spans="1:33" customFormat="false">
+    <row r="17" spans="1:32" customFormat="false">
       <c r="A17" s="0" t="inlineStr">
         <is>
           <t>Kab. Aceh Jaya</t>
@@ -20523,22 +20526,22 @@
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
-      <c r="H17" s="0" t="inlineStr">
+      <c r="H17" s="0"/>
+      <c r="I17" s="0" t="inlineStr">
         <is>
           <t>Kab. Bekasi</t>
         </is>
       </c>
-      <c r="I17" s="0" t="inlineStr">
+      <c r="J17" s="0" t="inlineStr">
         <is>
           <t>Kab. Blora</t>
         </is>
       </c>
-      <c r="J17" s="0" t="inlineStr">
+      <c r="K17" s="0" t="inlineStr">
         <is>
           <t>Kab. Mojokerto</t>
         </is>
       </c>
-      <c r="K17" s="0"/>
       <c r="L17" s="0"/>
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
@@ -20561,36 +20564,35 @@
       </c>
       <c r="X17" s="0"/>
       <c r="Y17" s="0"/>
-      <c r="Z17" s="0"/>
-      <c r="AA17" s="0" t="inlineStr">
+      <c r="Z17" s="0" t="inlineStr">
         <is>
           <t>Kab. Enrekang</t>
         </is>
       </c>
-      <c r="AB17" s="0"/>
-      <c r="AC17" s="0" t="inlineStr">
+      <c r="AA17" s="0"/>
+      <c r="AB17" s="0" t="inlineStr">
         <is>
           <t>Kendari</t>
         </is>
       </c>
-      <c r="AD17" s="0"/>
+      <c r="AC17" s="0"/>
+      <c r="AD17" s="0" t="inlineStr">
+        <is>
+          <t>Padang Panjang</t>
+        </is>
+      </c>
       <c r="AE17" s="0" t="inlineStr">
         <is>
-          <t>Padang Panjang</t>
+          <t>Pagar Alam</t>
         </is>
       </c>
       <c r="AF17" s="0" t="inlineStr">
         <is>
-          <t>Pagar Alam</t>
-        </is>
-      </c>
-      <c r="AG17" s="0" t="inlineStr">
-        <is>
           <t>Kab. Pakpak Bharat</t>
         </is>
       </c>
     </row>
-    <row r="18" spans="1:33" customFormat="false">
+    <row r="18" spans="1:32" customFormat="false">
       <c r="A18" s="0" t="inlineStr">
         <is>
           <t>Kab. Bener Meriah</t>
@@ -20602,22 +20604,22 @@
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
-      <c r="H18" s="0" t="inlineStr">
+      <c r="H18" s="0"/>
+      <c r="I18" s="0" t="inlineStr">
         <is>
           <t>Kab. Bandung Barat</t>
         </is>
       </c>
-      <c r="I18" s="0" t="inlineStr">
+      <c r="J18" s="0" t="inlineStr">
         <is>
           <t>Kab. Rembang</t>
         </is>
       </c>
-      <c r="J18" s="0" t="inlineStr">
+      <c r="K18" s="0" t="inlineStr">
         <is>
           <t>Kab. Jombang</t>
         </is>
       </c>
-      <c r="K18" s="0"/>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
@@ -20640,36 +20642,35 @@
       </c>
       <c r="X18" s="0"/>
       <c r="Y18" s="0"/>
-      <c r="Z18" s="0"/>
-      <c r="AA18" s="0" t="inlineStr">
+      <c r="Z18" s="0" t="inlineStr">
         <is>
           <t>Kab. Luwu</t>
         </is>
       </c>
-      <c r="AB18" s="0"/>
-      <c r="AC18" s="0" t="inlineStr">
+      <c r="AA18" s="0"/>
+      <c r="AB18" s="0" t="inlineStr">
         <is>
           <t>Babau</t>
         </is>
       </c>
-      <c r="AD18" s="0"/>
+      <c r="AC18" s="0"/>
+      <c r="AD18" s="0" t="inlineStr">
+        <is>
+          <t>Bukittinggi</t>
+        </is>
+      </c>
       <c r="AE18" s="0" t="inlineStr">
         <is>
-          <t>Bukittinggi</t>
+          <t>Lubuklinggau</t>
         </is>
       </c>
       <c r="AF18" s="0" t="inlineStr">
         <is>
-          <t>Lubuklinggau</t>
-        </is>
-      </c>
-      <c r="AG18" s="0" t="inlineStr">
-        <is>
           <t>Kab. Samosir</t>
         </is>
       </c>
     </row>
-    <row r="19" spans="1:33" customFormat="false">
+    <row r="19" spans="1:32" customFormat="false">
       <c r="A19" s="0" t="inlineStr">
         <is>
           <t>Kab. Pidie Jaya</t>
@@ -20681,22 +20682,22 @@
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
-      <c r="H19" s="0" t="inlineStr">
+      <c r="H19" s="0"/>
+      <c r="I19" s="0" t="inlineStr">
         <is>
           <t>Kab. Pangandaran</t>
         </is>
       </c>
-      <c r="I19" s="0" t="inlineStr">
+      <c r="J19" s="0" t="inlineStr">
         <is>
           <t>Kab. Pati</t>
         </is>
       </c>
-      <c r="J19" s="0" t="inlineStr">
+      <c r="K19" s="0" t="inlineStr">
         <is>
           <t>Kab. Nganjuk</t>
         </is>
       </c>
-      <c r="K19" s="0"/>
       <c r="L19" s="0"/>
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
@@ -20719,28 +20720,27 @@
       </c>
       <c r="X19" s="0"/>
       <c r="Y19" s="0"/>
-      <c r="Z19" s="0"/>
-      <c r="AA19" s="0" t="inlineStr">
+      <c r="Z19" s="0" t="inlineStr">
         <is>
           <t>Kab. Tana Toraja</t>
         </is>
       </c>
+      <c r="AA19" s="0"/>
       <c r="AB19" s="0"/>
       <c r="AC19" s="0"/>
-      <c r="AD19" s="0"/>
-      <c r="AE19" s="0" t="inlineStr">
+      <c r="AD19" s="0" t="inlineStr">
         <is>
           <t>Payakumbuh</t>
         </is>
       </c>
-      <c r="AF19" s="0"/>
-      <c r="AG19" s="0" t="inlineStr">
+      <c r="AE19" s="0"/>
+      <c r="AF19" s="0" t="inlineStr">
         <is>
           <t>Kab. Serdang Bedagai</t>
         </is>
       </c>
     </row>
-    <row r="20" spans="1:33" customFormat="false">
+    <row r="20" spans="1:32" customFormat="false">
       <c r="A20" s="0" t="inlineStr">
         <is>
           <t>Banda Aceh</t>
@@ -20752,22 +20752,22 @@
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
-      <c r="H20" s="0" t="inlineStr">
+      <c r="H20" s="0"/>
+      <c r="I20" s="0" t="inlineStr">
         <is>
           <t>Bogor</t>
         </is>
       </c>
-      <c r="I20" s="0" t="inlineStr">
+      <c r="J20" s="0" t="inlineStr">
         <is>
           <t>Kab. Kudus</t>
         </is>
       </c>
-      <c r="J20" s="0" t="inlineStr">
+      <c r="K20" s="0" t="inlineStr">
         <is>
           <t>Kab. Madiun</t>
         </is>
       </c>
-      <c r="K20" s="0"/>
       <c r="L20" s="0"/>
       <c r="M20" s="0"/>
       <c r="N20" s="0"/>
@@ -20790,28 +20790,27 @@
       </c>
       <c r="X20" s="0"/>
       <c r="Y20" s="0"/>
-      <c r="Z20" s="0"/>
-      <c r="AA20" s="0" t="inlineStr">
+      <c r="Z20" s="0" t="inlineStr">
         <is>
           <t>Kab. Luwu Utara</t>
         </is>
       </c>
+      <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
-      <c r="AD20" s="0"/>
-      <c r="AE20" s="0" t="inlineStr">
+      <c r="AD20" s="0" t="inlineStr">
         <is>
           <t>Pariaman</t>
         </is>
       </c>
-      <c r="AF20" s="0"/>
-      <c r="AG20" s="0" t="inlineStr">
+      <c r="AE20" s="0"/>
+      <c r="AF20" s="0" t="inlineStr">
         <is>
           <t>Kab. Batu Bara</t>
         </is>
       </c>
     </row>
-    <row r="21" spans="1:33" customFormat="false">
+    <row r="21" spans="1:32" customFormat="false">
       <c r="A21" s="0" t="inlineStr">
         <is>
           <t>Sabang</t>
@@ -20823,22 +20822,22 @@
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
-      <c r="H21" s="0" t="inlineStr">
+      <c r="H21" s="0"/>
+      <c r="I21" s="0" t="inlineStr">
         <is>
           <t>Sukabumi</t>
         </is>
       </c>
-      <c r="I21" s="0" t="inlineStr">
+      <c r="J21" s="0" t="inlineStr">
         <is>
           <t>Kab. Jepara</t>
         </is>
       </c>
-      <c r="J21" s="0" t="inlineStr">
+      <c r="K21" s="0" t="inlineStr">
         <is>
           <t>Kab. Magetan</t>
         </is>
       </c>
-      <c r="K21" s="0"/>
       <c r="L21" s="0"/>
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
@@ -20861,24 +20860,23 @@
       </c>
       <c r="X21" s="0"/>
       <c r="Y21" s="0"/>
-      <c r="Z21" s="0"/>
-      <c r="AA21" s="0" t="inlineStr">
+      <c r="Z21" s="0" t="inlineStr">
         <is>
           <t>Kab. Luwu Timur</t>
         </is>
       </c>
+      <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
       <c r="AC21" s="0"/>
       <c r="AD21" s="0"/>
       <c r="AE21" s="0"/>
-      <c r="AF21" s="0"/>
-      <c r="AG21" s="0" t="inlineStr">
+      <c r="AF21" s="0" t="inlineStr">
         <is>
           <t>Kab. Padang Lawas Utara</t>
         </is>
       </c>
     </row>
-    <row r="22" spans="1:33" customFormat="false">
+    <row r="22" spans="1:32" customFormat="false">
       <c r="A22" s="0" t="inlineStr">
         <is>
           <t>Langsa</t>
@@ -20890,22 +20888,22 @@
       <c r="E22" s="0"/>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
-      <c r="H22" s="0" t="inlineStr">
+      <c r="H22" s="0"/>
+      <c r="I22" s="0" t="inlineStr">
         <is>
           <t>Bandung</t>
         </is>
       </c>
-      <c r="I22" s="0" t="inlineStr">
+      <c r="J22" s="0" t="inlineStr">
         <is>
           <t>Kab. Demak</t>
         </is>
       </c>
-      <c r="J22" s="0" t="inlineStr">
+      <c r="K22" s="0" t="inlineStr">
         <is>
           <t>Kab. Ngawi</t>
         </is>
       </c>
-      <c r="K22" s="0"/>
       <c r="L22" s="0"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
@@ -20928,24 +20926,23 @@
       </c>
       <c r="X22" s="0"/>
       <c r="Y22" s="0"/>
-      <c r="Z22" s="0"/>
-      <c r="AA22" s="0" t="inlineStr">
+      <c r="Z22" s="0" t="inlineStr">
         <is>
           <t>Kab. Toraja Utara</t>
         </is>
       </c>
+      <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
       <c r="AC22" s="0"/>
       <c r="AD22" s="0"/>
       <c r="AE22" s="0"/>
-      <c r="AF22" s="0"/>
-      <c r="AG22" s="0" t="inlineStr">
+      <c r="AF22" s="0" t="inlineStr">
         <is>
           <t>Kab. Padang Lawas</t>
         </is>
       </c>
     </row>
-    <row r="23" spans="1:33" customFormat="false">
+    <row r="23" spans="1:32" customFormat="false">
       <c r="A23" s="0" t="inlineStr">
         <is>
           <t>Lhokseumawe</t>
@@ -20957,22 +20954,22 @@
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
-      <c r="H23" s="0" t="inlineStr">
+      <c r="H23" s="0"/>
+      <c r="I23" s="0" t="inlineStr">
         <is>
           <t>Cirebon</t>
         </is>
       </c>
-      <c r="I23" s="0" t="inlineStr">
+      <c r="J23" s="0" t="inlineStr">
         <is>
           <t>Kab. Semarang</t>
         </is>
       </c>
-      <c r="J23" s="0" t="inlineStr">
+      <c r="K23" s="0" t="inlineStr">
         <is>
           <t>Kab. Bojonegor</t>
         </is>
       </c>
-      <c r="K23" s="0"/>
       <c r="L23" s="0"/>
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
@@ -20995,24 +20992,23 @@
       </c>
       <c r="X23" s="0"/>
       <c r="Y23" s="0"/>
-      <c r="Z23" s="0"/>
-      <c r="AA23" s="0" t="inlineStr">
+      <c r="Z23" s="0" t="inlineStr">
         <is>
           <t>Makassar</t>
         </is>
       </c>
+      <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
       <c r="AC23" s="0"/>
       <c r="AD23" s="0"/>
       <c r="AE23" s="0"/>
-      <c r="AF23" s="0"/>
-      <c r="AG23" s="0" t="inlineStr">
+      <c r="AF23" s="0" t="inlineStr">
         <is>
           <t>Kab. Labuhan Batu Selatan</t>
         </is>
       </c>
     </row>
-    <row r="24" spans="1:33" customFormat="false">
+    <row r="24" spans="1:32" customFormat="false">
       <c r="A24" s="0" t="inlineStr">
         <is>
           <t>Subulussalam</t>
@@ -21024,22 +21020,22 @@
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
-      <c r="H24" s="0" t="inlineStr">
+      <c r="H24" s="0"/>
+      <c r="I24" s="0" t="inlineStr">
         <is>
           <t>Bekasi</t>
         </is>
       </c>
-      <c r="I24" s="0" t="inlineStr">
+      <c r="J24" s="0" t="inlineStr">
         <is>
           <t>Kab. Temanggung</t>
         </is>
       </c>
-      <c r="J24" s="0" t="inlineStr">
+      <c r="K24" s="0" t="inlineStr">
         <is>
           <t>Kab. Tuban</t>
         </is>
       </c>
-      <c r="K24" s="0"/>
       <c r="L24" s="0"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
@@ -21058,24 +21054,23 @@
       </c>
       <c r="X24" s="0"/>
       <c r="Y24" s="0"/>
-      <c r="Z24" s="0"/>
-      <c r="AA24" s="0" t="inlineStr">
+      <c r="Z24" s="0" t="inlineStr">
         <is>
           <t>Parepare</t>
         </is>
       </c>
+      <c r="AA24" s="0"/>
       <c r="AB24" s="0"/>
       <c r="AC24" s="0"/>
       <c r="AD24" s="0"/>
       <c r="AE24" s="0"/>
-      <c r="AF24" s="0"/>
-      <c r="AG24" s="0" t="inlineStr">
+      <c r="AF24" s="0" t="inlineStr">
         <is>
           <t>Kab. Labuhan Batu Utara</t>
         </is>
       </c>
     </row>
-    <row r="25" spans="1:33" customFormat="false">
+    <row r="25" spans="1:32" customFormat="false">
       <c r="A25" s="0"/>
       <c r="B25" s="0"/>
       <c r="C25" s="0"/>
@@ -21083,22 +21078,22 @@
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
-      <c r="H25" s="0" t="inlineStr">
+      <c r="H25" s="0"/>
+      <c r="I25" s="0" t="inlineStr">
         <is>
           <t>Depok</t>
         </is>
       </c>
-      <c r="I25" s="0" t="inlineStr">
+      <c r="J25" s="0" t="inlineStr">
         <is>
           <t>Kab. Kendal</t>
         </is>
       </c>
-      <c r="J25" s="0" t="inlineStr">
+      <c r="K25" s="0" t="inlineStr">
         <is>
           <t>Kab. Lamongan</t>
         </is>
       </c>
-      <c r="K25" s="0"/>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
@@ -21117,24 +21112,23 @@
       </c>
       <c r="X25" s="0"/>
       <c r="Y25" s="0"/>
-      <c r="Z25" s="0"/>
-      <c r="AA25" s="0" t="inlineStr">
+      <c r="Z25" s="0" t="inlineStr">
         <is>
           <t>Palopo</t>
         </is>
       </c>
+      <c r="AA25" s="0"/>
       <c r="AB25" s="0"/>
       <c r="AC25" s="0"/>
       <c r="AD25" s="0"/>
       <c r="AE25" s="0"/>
-      <c r="AF25" s="0"/>
-      <c r="AG25" s="0" t="inlineStr">
+      <c r="AF25" s="0" t="inlineStr">
         <is>
           <t>Kab. Nias Utara</t>
         </is>
       </c>
     </row>
-    <row r="26" spans="1:33" customFormat="false">
+    <row r="26" spans="1:32" customFormat="false">
       <c r="A26" s="0"/>
       <c r="B26" s="0"/>
       <c r="C26" s="0"/>
@@ -21142,22 +21136,22 @@
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
-      <c r="H26" s="0" t="inlineStr">
+      <c r="H26" s="0"/>
+      <c r="I26" s="0" t="inlineStr">
         <is>
           <t>Cimahi</t>
         </is>
       </c>
-      <c r="I26" s="0" t="inlineStr">
+      <c r="J26" s="0" t="inlineStr">
         <is>
           <t>Kab. Batang</t>
         </is>
       </c>
-      <c r="J26" s="0" t="inlineStr">
+      <c r="K26" s="0" t="inlineStr">
         <is>
           <t>Kab. Gresik</t>
         </is>
       </c>
-      <c r="K26" s="0"/>
       <c r="L26" s="0"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
@@ -21182,14 +21176,13 @@
       <c r="AC26" s="0"/>
       <c r="AD26" s="0"/>
       <c r="AE26" s="0"/>
-      <c r="AF26" s="0"/>
-      <c r="AG26" s="0" t="inlineStr">
+      <c r="AF26" s="0" t="inlineStr">
         <is>
           <t>Kab. Nias Barat</t>
         </is>
       </c>
     </row>
-    <row r="27" spans="1:33" customFormat="false">
+    <row r="27" spans="1:32" customFormat="false">
       <c r="A27" s="0"/>
       <c r="B27" s="0"/>
       <c r="C27" s="0"/>
@@ -21197,22 +21190,22 @@
       <c r="E27" s="0"/>
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
-      <c r="H27" s="0" t="inlineStr">
+      <c r="H27" s="0"/>
+      <c r="I27" s="0" t="inlineStr">
         <is>
           <t>Tasikmalaya</t>
         </is>
       </c>
-      <c r="I27" s="0" t="inlineStr">
+      <c r="J27" s="0" t="inlineStr">
         <is>
           <t>Kab. Pekalongan</t>
         </is>
       </c>
-      <c r="J27" s="0" t="inlineStr">
+      <c r="K27" s="0" t="inlineStr">
         <is>
           <t>Kab. Bangkalan</t>
         </is>
       </c>
-      <c r="K27" s="0"/>
       <c r="L27" s="0"/>
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
@@ -21237,14 +21230,13 @@
       <c r="AC27" s="0"/>
       <c r="AD27" s="0"/>
       <c r="AE27" s="0"/>
-      <c r="AF27" s="0"/>
-      <c r="AG27" s="0" t="inlineStr">
+      <c r="AF27" s="0" t="inlineStr">
         <is>
           <t>Sibolga</t>
         </is>
       </c>
     </row>
-    <row r="28" spans="1:33" customFormat="false">
+    <row r="28" spans="1:32" customFormat="false">
       <c r="A28" s="0"/>
       <c r="B28" s="0"/>
       <c r="C28" s="0"/>
@@ -21252,22 +21244,22 @@
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
-      <c r="H28" s="0" t="inlineStr">
+      <c r="H28" s="0"/>
+      <c r="I28" s="0" t="inlineStr">
         <is>
           <t>Banjar</t>
         </is>
       </c>
-      <c r="I28" s="0" t="inlineStr">
+      <c r="J28" s="0" t="inlineStr">
         <is>
           <t>Kab. Pemalang</t>
         </is>
       </c>
-      <c r="J28" s="0" t="inlineStr">
+      <c r="K28" s="0" t="inlineStr">
         <is>
           <t>Kab. Sampang</t>
         </is>
       </c>
-      <c r="K28" s="0"/>
       <c r="L28" s="0"/>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
@@ -21292,14 +21284,13 @@
       <c r="AC28" s="0"/>
       <c r="AD28" s="0"/>
       <c r="AE28" s="0"/>
-      <c r="AF28" s="0"/>
-      <c r="AG28" s="0" t="inlineStr">
+      <c r="AF28" s="0" t="inlineStr">
         <is>
           <t>Tanjung Balai</t>
         </is>
       </c>
     </row>
-    <row r="29" spans="1:33" customFormat="false">
+    <row r="29" spans="1:32" customFormat="false">
       <c r="A29" s="0"/>
       <c r="B29" s="0"/>
       <c r="C29" s="0"/>
@@ -21308,17 +21299,17 @@
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="0" t="inlineStr">
+      <c r="I29" s="0"/>
+      <c r="J29" s="0" t="inlineStr">
         <is>
           <t>Kab. Tegal</t>
         </is>
       </c>
-      <c r="J29" s="0" t="inlineStr">
+      <c r="K29" s="0" t="inlineStr">
         <is>
           <t>Kab. Pamekasan</t>
         </is>
       </c>
-      <c r="K29" s="0"/>
       <c r="L29" s="0"/>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
@@ -21343,14 +21334,13 @@
       <c r="AC29" s="0"/>
       <c r="AD29" s="0"/>
       <c r="AE29" s="0"/>
-      <c r="AF29" s="0"/>
-      <c r="AG29" s="0" t="inlineStr">
+      <c r="AF29" s="0" t="inlineStr">
         <is>
           <t>Pematang Siantar</t>
         </is>
       </c>
     </row>
-    <row r="30" spans="1:33" customFormat="false">
+    <row r="30" spans="1:32" customFormat="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0"/>
       <c r="C30" s="0"/>
@@ -21359,17 +21349,17 @@
       <c r="F30" s="0"/>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="0" t="inlineStr">
+      <c r="I30" s="0"/>
+      <c r="J30" s="0" t="inlineStr">
         <is>
           <t>Kab. Brebes</t>
         </is>
       </c>
-      <c r="J30" s="0" t="inlineStr">
+      <c r="K30" s="0" t="inlineStr">
         <is>
           <t>Kab. Sumenep</t>
         </is>
       </c>
-      <c r="K30" s="0"/>
       <c r="L30" s="0"/>
       <c r="M30" s="0"/>
       <c r="N30" s="0"/>
@@ -21394,14 +21384,13 @@
       <c r="AC30" s="0"/>
       <c r="AD30" s="0"/>
       <c r="AE30" s="0"/>
-      <c r="AF30" s="0"/>
-      <c r="AG30" s="0" t="inlineStr">
+      <c r="AF30" s="0" t="inlineStr">
         <is>
           <t>Tebing Tinggi</t>
         </is>
       </c>
     </row>
-    <row r="31" spans="1:33" customFormat="false">
+    <row r="31" spans="1:32" customFormat="false">
       <c r="A31" s="0"/>
       <c r="B31" s="0"/>
       <c r="C31" s="0"/>
@@ -21410,17 +21399,17 @@
       <c r="F31" s="0"/>
       <c r="G31" s="0"/>
       <c r="H31" s="0"/>
-      <c r="I31" s="0" t="inlineStr">
+      <c r="I31" s="0"/>
+      <c r="J31" s="0" t="inlineStr">
         <is>
           <t>Magelang</t>
         </is>
       </c>
-      <c r="J31" s="0" t="inlineStr">
+      <c r="K31" s="0" t="inlineStr">
         <is>
           <t>Kediri</t>
         </is>
       </c>
-      <c r="K31" s="0"/>
       <c r="L31" s="0"/>
       <c r="M31" s="0"/>
       <c r="N31" s="0"/>
@@ -21441,14 +21430,13 @@
       <c r="AC31" s="0"/>
       <c r="AD31" s="0"/>
       <c r="AE31" s="0"/>
-      <c r="AF31" s="0"/>
-      <c r="AG31" s="0" t="inlineStr">
+      <c r="AF31" s="0" t="inlineStr">
         <is>
           <t>Medan</t>
         </is>
       </c>
     </row>
-    <row r="32" spans="1:33" customFormat="false">
+    <row r="32" spans="1:32" customFormat="false">
       <c r="A32" s="0"/>
       <c r="B32" s="0"/>
       <c r="C32" s="0"/>
@@ -21457,17 +21445,17 @@
       <c r="F32" s="0"/>
       <c r="G32" s="0"/>
       <c r="H32" s="0"/>
-      <c r="I32" s="0" t="inlineStr">
+      <c r="I32" s="0"/>
+      <c r="J32" s="0" t="inlineStr">
         <is>
           <t>Surakarta</t>
         </is>
       </c>
-      <c r="J32" s="0" t="inlineStr">
+      <c r="K32" s="0" t="inlineStr">
         <is>
           <t>Blitar</t>
         </is>
       </c>
-      <c r="K32" s="0"/>
       <c r="L32" s="0"/>
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
@@ -21488,14 +21476,13 @@
       <c r="AC32" s="0"/>
       <c r="AD32" s="0"/>
       <c r="AE32" s="0"/>
-      <c r="AF32" s="0"/>
-      <c r="AG32" s="0" t="inlineStr">
+      <c r="AF32" s="0" t="inlineStr">
         <is>
           <t>Binjai</t>
         </is>
       </c>
     </row>
-    <row r="33" spans="1:33" customFormat="false">
+    <row r="33" spans="1:32" customFormat="false">
       <c r="A33" s="0"/>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -21504,17 +21491,17 @@
       <c r="F33" s="0"/>
       <c r="G33" s="0"/>
       <c r="H33" s="0"/>
-      <c r="I33" s="0" t="inlineStr">
+      <c r="I33" s="0"/>
+      <c r="J33" s="0" t="inlineStr">
         <is>
           <t>Salatiga</t>
         </is>
       </c>
-      <c r="J33" s="0" t="inlineStr">
+      <c r="K33" s="0" t="inlineStr">
         <is>
           <t>Malang</t>
         </is>
       </c>
-      <c r="K33" s="0"/>
       <c r="L33" s="0"/>
       <c r="M33" s="0"/>
       <c r="N33" s="0"/>
@@ -21535,14 +21522,13 @@
       <c r="AC33" s="0"/>
       <c r="AD33" s="0"/>
       <c r="AE33" s="0"/>
-      <c r="AF33" s="0"/>
-      <c r="AG33" s="0" t="inlineStr">
+      <c r="AF33" s="0" t="inlineStr">
         <is>
           <t>Padangsidimpuan</t>
         </is>
       </c>
     </row>
-    <row r="34" spans="1:33" customFormat="false">
+    <row r="34" spans="1:32" customFormat="false">
       <c r="A34" s="0"/>
       <c r="B34" s="0"/>
       <c r="C34" s="0"/>
@@ -21551,17 +21537,17 @@
       <c r="F34" s="0"/>
       <c r="G34" s="0"/>
       <c r="H34" s="0"/>
-      <c r="I34" s="0" t="inlineStr">
+      <c r="I34" s="0"/>
+      <c r="J34" s="0" t="inlineStr">
         <is>
           <t>Semarang</t>
         </is>
       </c>
-      <c r="J34" s="0" t="inlineStr">
+      <c r="K34" s="0" t="inlineStr">
         <is>
           <t>Probolinggo</t>
         </is>
       </c>
-      <c r="K34" s="0"/>
       <c r="L34" s="0"/>
       <c r="M34" s="0"/>
       <c r="N34" s="0"/>
@@ -21582,14 +21568,13 @@
       <c r="AC34" s="0"/>
       <c r="AD34" s="0"/>
       <c r="AE34" s="0"/>
-      <c r="AF34" s="0"/>
-      <c r="AG34" s="0" t="inlineStr">
+      <c r="AF34" s="0" t="inlineStr">
         <is>
           <t>Gunungsitoli</t>
         </is>
       </c>
     </row>
-    <row r="35" spans="1:10" customFormat="false">
+    <row r="35" spans="1:11" customFormat="false">
       <c r="A35" s="0"/>
       <c r="B35" s="0"/>
       <c r="C35" s="0"/>
@@ -21598,18 +21583,19 @@
       <c r="F35" s="0"/>
       <c r="G35" s="0"/>
       <c r="H35" s="0"/>
-      <c r="I35" s="0" t="inlineStr">
+      <c r="I35" s="0"/>
+      <c r="J35" s="0" t="inlineStr">
         <is>
           <t>Pekalongan</t>
         </is>
       </c>
-      <c r="J35" s="0" t="inlineStr">
+      <c r="K35" s="0" t="inlineStr">
         <is>
           <t>Pasuruan</t>
         </is>
       </c>
     </row>
-    <row r="36" spans="1:10" customFormat="false">
+    <row r="36" spans="1:11" customFormat="false">
       <c r="A36" s="0"/>
       <c r="B36" s="0"/>
       <c r="C36" s="0"/>
@@ -21618,12 +21604,13 @@
       <c r="F36" s="0"/>
       <c r="G36" s="0"/>
       <c r="H36" s="0"/>
-      <c r="I36" s="0" t="inlineStr">
+      <c r="I36" s="0"/>
+      <c r="J36" s="0" t="inlineStr">
         <is>
           <t>Tegal</t>
         </is>
       </c>
-      <c r="J36" s="0" t="inlineStr">
+      <c r="K36" s="0" t="inlineStr">
         <is>
           <t>Mojokerto</t>
         </is>

</xml_diff>